<commit_message>
set up test file
</commit_message>
<xml_diff>
--- a/tests/frameworks/framework_sir.xlsx
+++ b/tests/frameworks/framework_sir.xlsx
@@ -5,11 +5,11 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/robynstuart/Documents/git/core/tests/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/robynstuart/Documents/git/optimacore/tests/frameworks/"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="240" yWindow="460" windowWidth="28560" windowHeight="16640" activeTab="1"/>
+    <workbookView xWindow="240" yWindow="460" windowWidth="28560" windowHeight="16640" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="Instructions" sheetId="6" r:id="rId1"/>
@@ -17,6 +17,7 @@
     <sheet name="Transitions" sheetId="3" r:id="rId3"/>
     <sheet name="Characteristics" sheetId="4" r:id="rId4"/>
     <sheet name="Parameters" sheetId="5" r:id="rId5"/>
+    <sheet name="Program Types" sheetId="7" r:id="rId6"/>
   </sheets>
   <calcPr calcId="150001" concurrentCalc="0"/>
   <extLst>
@@ -313,7 +314,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="124" uniqueCount="71">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="103" uniqueCount="68">
   <si>
     <t>Display Name</t>
   </si>
@@ -375,21 +376,6 @@
     <t>Default Value</t>
   </si>
   <si>
-    <t>noneed</t>
-  </si>
-  <si>
-    <t>unaware</t>
-  </si>
-  <si>
-    <t>unlinked</t>
-  </si>
-  <si>
-    <t>unsuccess</t>
-  </si>
-  <si>
-    <t>success</t>
-  </si>
-  <si>
     <t>death</t>
   </si>
   <si>
@@ -405,63 +391,6 @@
     <t>failrate</t>
   </si>
   <si>
-    <t>All people with need</t>
-  </si>
-  <si>
-    <t>All people aware of need</t>
-  </si>
-  <si>
-    <t>All people linked to services</t>
-  </si>
-  <si>
-    <t>All people with successful outcomes</t>
-  </si>
-  <si>
-    <t>ch_need</t>
-  </si>
-  <si>
-    <t>ch_aware</t>
-  </si>
-  <si>
-    <t>ch_linked</t>
-  </si>
-  <si>
-    <t>ch_success</t>
-  </si>
-  <si>
-    <t>success, unsuccess</t>
-  </si>
-  <si>
-    <t>ch_linked, unlinked</t>
-  </si>
-  <si>
-    <t>ch_aware, unaware</t>
-  </si>
-  <si>
-    <t>Proportion with successful outcomes</t>
-  </si>
-  <si>
-    <t>ch_propsuccess</t>
-  </si>
-  <si>
-    <t>ch_proplinked</t>
-  </si>
-  <si>
-    <t>ch_propaware</t>
-  </si>
-  <si>
-    <t>ch_propneed</t>
-  </si>
-  <si>
-    <t>Proportion linked to services</t>
-  </si>
-  <si>
-    <t>Proportion aware of need</t>
-  </si>
-  <si>
-    <t>Proportion with need</t>
-  </si>
-  <si>
     <t>Number of people acquiring need annually</t>
   </si>
   <si>
@@ -526,6 +455,69 @@
   </si>
   <si>
     <t>Dead</t>
+  </si>
+  <si>
+    <t>sus</t>
+  </si>
+  <si>
+    <t>inf</t>
+  </si>
+  <si>
+    <t>rec</t>
+  </si>
+  <si>
+    <t>dead</t>
+  </si>
+  <si>
+    <t>rec_rate</t>
+  </si>
+  <si>
+    <t>foi</t>
+  </si>
+  <si>
+    <t>sus_death</t>
+  </si>
+  <si>
+    <t>inf_death</t>
+  </si>
+  <si>
+    <t>Number ever infected</t>
+  </si>
+  <si>
+    <t>inf, rec</t>
+  </si>
+  <si>
+    <t>Number infected or susceptible</t>
+  </si>
+  <si>
+    <t>ch_infsus</t>
+  </si>
+  <si>
+    <t>ch_infrec</t>
+  </si>
+  <si>
+    <t>ch_newinf</t>
+  </si>
+  <si>
+    <t>inf, sus</t>
+  </si>
+  <si>
+    <t>sus, rec</t>
+  </si>
+  <si>
+    <t>Number not at risk of infection</t>
+  </si>
+  <si>
+    <t>Proportion ever infected</t>
+  </si>
+  <si>
+    <t>Proportion infected or susceptible</t>
+  </si>
+  <si>
+    <t>Proportion not at risk of infection</t>
+  </si>
+  <si>
+    <t>sus, inf, rec</t>
   </si>
 </sst>
 </file>
@@ -1260,29 +1252,29 @@
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A1" s="4" t="s">
-        <v>59</v>
+        <v>35</v>
       </c>
       <c r="B1" t="s">
-        <v>60</v>
+        <v>36</v>
       </c>
       <c r="C1" s="11">
         <f ca="1">TODAY()</f>
-        <v>43182</v>
+        <v>43183</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>62</v>
+        <v>38</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>63</v>
+        <v>39</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>64</v>
+        <v>40</v>
       </c>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.2">
@@ -1316,8 +1308,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E7"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="169" zoomScaleNormal="127" workbookViewId="0">
-      <selection activeCell="C4" sqref="C4"/>
+    <sheetView zoomScale="169" zoomScaleNormal="127" workbookViewId="0">
+      <selection activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -1345,10 +1337,10 @@
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A2" s="2" t="s">
-        <v>67</v>
+        <v>43</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>20</v>
+        <v>47</v>
       </c>
       <c r="C2" s="2" t="s">
         <v>7</v>
@@ -1362,10 +1354,10 @@
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A3" s="2" t="s">
-        <v>68</v>
+        <v>44</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>21</v>
+        <v>48</v>
       </c>
       <c r="C3" s="2" t="s">
         <v>5</v>
@@ -1379,10 +1371,10 @@
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A4" s="2" t="s">
-        <v>69</v>
+        <v>45</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>22</v>
+        <v>49</v>
       </c>
       <c r="C4" s="2" t="s">
         <v>5</v>
@@ -1396,10 +1388,10 @@
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A5" s="2" t="s">
-        <v>70</v>
+        <v>46</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>23</v>
+        <v>50</v>
       </c>
       <c r="C5" s="2" t="s">
         <v>5</v>
@@ -1438,10 +1430,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:I8"/>
+  <dimension ref="A1:G7"/>
   <sheetViews>
     <sheetView zoomScale="171" zoomScaleNormal="224" workbookViewId="0">
-      <selection activeCell="I2" sqref="I2:I8"/>
+      <selection activeCell="D5" sqref="D5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -1455,126 +1447,70 @@
     <col min="7" max="7" width="11" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.2">
       <c r="B1" s="1" t="str">
         <f>Compartments!B2</f>
-        <v>noneed</v>
+        <v>sus</v>
       </c>
       <c r="C1" s="1" t="str">
         <f>Compartments!B3</f>
-        <v>unaware</v>
+        <v>inf</v>
       </c>
       <c r="D1" s="1" t="str">
         <f>Compartments!B4</f>
-        <v>unlinked</v>
+        <v>rec</v>
       </c>
       <c r="E1" s="1" t="str">
         <f>Compartments!B5</f>
-        <v>unsuccess</v>
-      </c>
-      <c r="F1" s="1">
-        <f>Compartments!B6</f>
-        <v>0</v>
-      </c>
-      <c r="G1" s="1">
-        <f>Compartments!B7</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.2">
+        <v>dead</v>
+      </c>
+      <c r="F1" s="1"/>
+      <c r="G1" s="1"/>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A2" s="1" t="str">
         <f>Compartments!B2</f>
-        <v>noneed</v>
+        <v>sus</v>
       </c>
       <c r="C2" t="s">
-        <v>8</v>
-      </c>
-      <c r="G2" t="s">
-        <v>25</v>
-      </c>
-      <c r="I2" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.2">
+        <v>52</v>
+      </c>
+      <c r="E2" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A3" s="1" t="str">
         <f>Compartments!B3</f>
-        <v>unaware</v>
+        <v>inf</v>
       </c>
       <c r="D3" t="s">
-        <v>52</v>
-      </c>
-      <c r="G3" t="s">
-        <v>25</v>
-      </c>
-      <c r="I3" t="s">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.2">
+        <v>51</v>
+      </c>
+      <c r="E3" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A4" s="1" t="str">
         <f>Compartments!B4</f>
-        <v>unlinked</v>
+        <v>rec</v>
       </c>
       <c r="E4" t="s">
-        <v>26</v>
-      </c>
-      <c r="G4" t="s">
-        <v>25</v>
-      </c>
-      <c r="I4" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.2">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A5" s="1" t="str">
         <f>Compartments!B5</f>
-        <v>unsuccess</v>
-      </c>
-      <c r="D5" t="s">
-        <v>27</v>
-      </c>
-      <c r="F5" t="s">
-        <v>28</v>
-      </c>
-      <c r="G5" t="s">
-        <v>25</v>
-      </c>
-      <c r="I5" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A6" s="1">
-        <f>Compartments!B6</f>
-        <v>0</v>
-      </c>
-      <c r="D6" t="s">
-        <v>27</v>
-      </c>
-      <c r="E6" t="s">
-        <v>29</v>
-      </c>
-      <c r="G6" t="s">
-        <v>25</v>
-      </c>
-      <c r="I6" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A7" s="1">
-        <f>Compartments!B7</f>
-        <v>0</v>
-      </c>
-      <c r="I7" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="I8" t="s">
-        <v>25</v>
-      </c>
+        <v>dead</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A6" s="1"/>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A7" s="1"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -1585,8 +1521,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F20"/>
   <sheetViews>
-    <sheetView zoomScale="183" workbookViewId="0">
-      <selection activeCell="E6" sqref="E6"/>
+    <sheetView tabSelected="1" zoomScale="189" workbookViewId="0">
+      <selection activeCell="D7" sqref="D7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -1619,13 +1555,13 @@
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A2" s="6" t="s">
-        <v>33</v>
+        <v>55</v>
       </c>
       <c r="B2" s="6" t="s">
-        <v>37</v>
+        <v>59</v>
       </c>
       <c r="C2" s="6" t="s">
-        <v>24</v>
+        <v>56</v>
       </c>
       <c r="D2" s="6"/>
       <c r="E2" s="6"/>
@@ -1633,13 +1569,13 @@
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A3" s="6" t="s">
-        <v>32</v>
+        <v>57</v>
       </c>
       <c r="B3" s="6" t="s">
-        <v>36</v>
+        <v>58</v>
       </c>
       <c r="C3" s="6" t="s">
-        <v>38</v>
+        <v>61</v>
       </c>
       <c r="D3" s="6"/>
       <c r="E3" s="6"/>
@@ -1647,13 +1583,13 @@
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A4" s="6" t="s">
-        <v>31</v>
+        <v>63</v>
       </c>
       <c r="B4" s="6" t="s">
-        <v>35</v>
+        <v>60</v>
       </c>
       <c r="C4" s="6" t="s">
-        <v>39</v>
+        <v>62</v>
       </c>
       <c r="D4" s="6"/>
       <c r="E4" s="6"/>
@@ -1661,80 +1597,66 @@
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A5" s="6" t="s">
-        <v>30</v>
+        <v>64</v>
       </c>
       <c r="B5" s="6" t="s">
-        <v>34</v>
+        <v>59</v>
       </c>
       <c r="C5" s="6" t="s">
-        <v>40</v>
+        <v>56</v>
       </c>
       <c r="D5" s="6"/>
-      <c r="E5" s="6"/>
+      <c r="E5" s="6" t="s">
+        <v>67</v>
+      </c>
       <c r="F5" s="6"/>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A6" s="6" t="s">
-        <v>41</v>
+        <v>65</v>
       </c>
       <c r="B6" s="6" t="s">
-        <v>42</v>
+        <v>58</v>
       </c>
       <c r="C6" s="6" t="s">
-        <v>24</v>
+        <v>61</v>
       </c>
       <c r="D6" s="6"/>
       <c r="E6" s="6" t="s">
-        <v>34</v>
+        <v>67</v>
       </c>
       <c r="F6" s="6"/>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A7" s="6" t="s">
-        <v>46</v>
+        <v>66</v>
       </c>
       <c r="B7" s="6" t="s">
-        <v>43</v>
+        <v>60</v>
       </c>
       <c r="C7" s="6" t="s">
-        <v>38</v>
+        <v>62</v>
       </c>
       <c r="D7" s="6"/>
       <c r="E7" s="6" t="s">
-        <v>34</v>
+        <v>67</v>
       </c>
       <c r="F7" s="6"/>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A8" s="6" t="s">
-        <v>47</v>
-      </c>
-      <c r="B8" s="6" t="s">
-        <v>44</v>
-      </c>
-      <c r="C8" s="6" t="s">
-        <v>39</v>
-      </c>
+      <c r="A8" s="6"/>
+      <c r="B8" s="6"/>
+      <c r="C8" s="6"/>
       <c r="D8" s="6"/>
-      <c r="E8" s="6" t="s">
-        <v>34</v>
-      </c>
+      <c r="E8" s="6"/>
       <c r="F8" s="6"/>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A9" s="6" t="s">
-        <v>48</v>
-      </c>
-      <c r="B9" s="6" t="s">
-        <v>45</v>
-      </c>
-      <c r="C9" s="6" t="s">
-        <v>40</v>
-      </c>
+      <c r="A9" s="6"/>
+      <c r="B9" s="6"/>
+      <c r="C9" s="6"/>
       <c r="D9" s="6"/>
-      <c r="E9" s="6" t="s">
-        <v>34</v>
-      </c>
+      <c r="E9" s="6"/>
       <c r="F9" s="6"/>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.2">
@@ -1822,12 +1744,12 @@
         <v>19</v>
       </c>
       <c r="F1" s="9" t="s">
-        <v>61</v>
+        <v>37</v>
       </c>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A2" s="5" t="s">
-        <v>49</v>
+        <v>25</v>
       </c>
       <c r="B2" s="6" t="s">
         <v>8</v>
@@ -1839,7 +1761,7 @@
         <v>100</v>
       </c>
       <c r="F2" s="10" t="s">
-        <v>65</v>
+        <v>41</v>
       </c>
       <c r="H2" t="s">
         <v>8</v>
@@ -1847,7 +1769,7 @@
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A3" s="5" t="s">
-        <v>53</v>
+        <v>29</v>
       </c>
       <c r="B3" s="6" t="s">
         <v>9</v>
@@ -1856,10 +1778,10 @@
         <v>13</v>
       </c>
       <c r="F3" s="10" t="s">
-        <v>65</v>
+        <v>41</v>
       </c>
       <c r="H3" t="s">
-        <v>52</v>
+        <v>28</v>
       </c>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.2">
@@ -1867,75 +1789,75 @@
         <v>14</v>
       </c>
       <c r="B4" s="6" t="s">
-        <v>51</v>
+        <v>27</v>
       </c>
       <c r="D4" t="s">
         <v>12</v>
       </c>
       <c r="F4" s="10" t="s">
-        <v>65</v>
+        <v>41</v>
       </c>
       <c r="H4" t="s">
-        <v>27</v>
+        <v>22</v>
       </c>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A5" s="5" t="s">
-        <v>54</v>
+        <v>30</v>
       </c>
       <c r="B5" s="6" t="s">
-        <v>27</v>
+        <v>22</v>
       </c>
       <c r="D5" t="s">
         <v>15</v>
       </c>
       <c r="F5" s="10" t="s">
-        <v>65</v>
+        <v>41</v>
       </c>
       <c r="H5" t="s">
-        <v>26</v>
+        <v>21</v>
       </c>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A6" s="5" t="s">
-        <v>55</v>
+        <v>31</v>
       </c>
       <c r="B6" s="6" t="s">
-        <v>56</v>
+        <v>32</v>
       </c>
       <c r="D6" t="s">
         <v>12</v>
       </c>
       <c r="F6" s="10" t="s">
-        <v>66</v>
+        <v>42</v>
       </c>
       <c r="H6" t="s">
-        <v>29</v>
+        <v>24</v>
       </c>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A7" s="5" t="s">
-        <v>57</v>
+        <v>33</v>
       </c>
       <c r="B7" s="6" t="s">
-        <v>58</v>
+        <v>34</v>
       </c>
       <c r="D7" t="s">
         <v>13</v>
       </c>
       <c r="F7" s="10" t="s">
-        <v>66</v>
+        <v>42</v>
       </c>
       <c r="H7" t="s">
-        <v>28</v>
+        <v>23</v>
       </c>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A8" s="5" t="s">
-        <v>50</v>
+        <v>26</v>
       </c>
       <c r="B8" s="6" t="s">
-        <v>25</v>
+        <v>20</v>
       </c>
       <c r="D8" t="s">
         <v>13</v>
@@ -1944,10 +1866,10 @@
         <v>0.02</v>
       </c>
       <c r="F8" s="10" t="s">
-        <v>66</v>
+        <v>42</v>
       </c>
       <c r="H8" t="s">
-        <v>25</v>
+        <v>20</v>
       </c>
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.2">
@@ -1986,4 +1908,16 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <legacyDrawing r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetData/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
more conversion to odicts
</commit_message>
<xml_diff>
--- a/tests/frameworks/framework_sir.xlsx
+++ b/tests/frameworks/framework_sir.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="240" yWindow="460" windowWidth="28560" windowHeight="16640" activeTab="4"/>
+    <workbookView xWindow="240" yWindow="460" windowWidth="28560" windowHeight="16640" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="Instructions" sheetId="6" r:id="rId1"/>
@@ -1521,7 +1521,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F20"/>
   <sheetViews>
-    <sheetView zoomScale="189" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScale="189" workbookViewId="0">
       <selection activeCell="D7" sqref="D7"/>
     </sheetView>
   </sheetViews>
@@ -1714,7 +1714,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H16"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="160" workbookViewId="0">
+    <sheetView zoomScale="160" workbookViewId="0">
       <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
4hrs later, have finally loaded data
</commit_message>
<xml_diff>
--- a/tests/frameworks/framework_sir.xlsx
+++ b/tests/frameworks/framework_sir.xlsx
@@ -12,12 +12,11 @@
     <workbookView xWindow="240" yWindow="460" windowWidth="28560" windowHeight="16640" activeTab="3"/>
   </bookViews>
   <sheets>
-    <sheet name="Instructions" sheetId="6" r:id="rId1"/>
-    <sheet name="Compartments" sheetId="2" r:id="rId2"/>
-    <sheet name="Transitions" sheetId="3" r:id="rId3"/>
-    <sheet name="Characteristics" sheetId="4" r:id="rId4"/>
-    <sheet name="Parameters" sheetId="5" r:id="rId5"/>
-    <sheet name="Program Types" sheetId="7" r:id="rId6"/>
+    <sheet name="Compartments" sheetId="2" r:id="rId1"/>
+    <sheet name="Transitions" sheetId="3" r:id="rId2"/>
+    <sheet name="Characteristics" sheetId="4" r:id="rId3"/>
+    <sheet name="Parameters" sheetId="5" r:id="rId4"/>
+    <sheet name="Program Types" sheetId="7" r:id="rId5"/>
   </sheets>
   <calcPr calcId="150001" concurrentCalc="0"/>
   <extLst>
@@ -46,6 +45,31 @@
             <rFont val="Tahoma"/>
             <family val="2"/>
           </rPr>
+          <t>This column is for the 'code name' of a compartment within a
+population cascade, a state that an entity can exist in that is
+distinct from all other states.
+Examples may include 'sus', 'inf_1', 'rec', etc.
+If entities in the network involve two 'orthogonal' descriptors,
+compartments should combine the status of each state in the title,
+e.g. 'inc_high_edu_hs', to make sure that each entity in a cascade is
+only ever in one state at a time.
+It is possible to bundle independent states as analytical features of
+interest elsewhere in the framework file.
+Note: A code name is a representative key that developers interface
+with (e.g. in scripts and the codebase).
+It should be in lower case without spaces.</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="B1" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <sz val="8"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
           <t>This column is for the 'display name' of a compartment within a
 population cascade, a state that an entity can exist in that is
 distinct from all other states.
@@ -60,31 +84,6 @@
 Note: A display name is a representative label that users interface
 with (e.g. in databooks and plots).
 It should be in title or sentence case.</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="B1" authorId="0">
-      <text>
-        <r>
-          <rPr>
-            <sz val="8"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t>This column is for the 'code name' of a compartment within a
-population cascade, a state that an entity can exist in that is
-distinct from all other states.
-Examples may include 'sus', 'inf_1', 'rec', etc.
-If entities in the network involve two 'orthogonal' descriptors,
-compartments should combine the status of each state in the title,
-e.g. 'inc_high_edu_hs', to make sure that each entity in a cascade is
-only ever in one state at a time.
-It is possible to bundle independent states as analytical features of
-interest elsewhere in the framework file.
-Note: A code name is a representative key that developers interface
-with (e.g. in scripts and the codebase).
-It should be in lower case without spaces.</t>
         </r>
       </text>
     </comment>
@@ -186,6 +185,31 @@
             <rFont val="Tahoma"/>
             <family val="2"/>
           </rPr>
+          <t>This column is for the 'code name' of a cascade characteristic,
+which is a set of compartments or, recursively, other characteristics.
+While a characteristic value is typically the population size across
+a set of compartments at a point in time, it can also be normalized by
+another characteristic.
+Defining a characteristic allows the model to track other important
+system state variables beyond the size of just one compartment.
+Examples include 'alive', 'num_inf_all', 'prop_imm', etc.
+Importantly, each compartment defined elsewhere also serves as a
+characteristic.
+Note: A code name is a representative key that developers interface
+with (e.g. in scripts and the codebase).
+It should be in lower case without spaces.</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="B1" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <sz val="8"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
           <t>This column is for the 'display name' of a cascade characteristic,
 which is a set of compartments or, recursively, other characteristics.
 While a characteristic value is typically the population size across
@@ -200,31 +224,6 @@
 Note: A display name is a representative label that users interface
 with (e.g. in databooks and plots).
 It should be in title or sentence case.</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="B1" authorId="0">
-      <text>
-        <r>
-          <rPr>
-            <sz val="8"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t>This column is for the 'code name' of a cascade characteristic,
-which is a set of compartments or, recursively, other characteristics.
-While a characteristic value is typically the population size across
-a set of compartments at a point in time, it can also be normalized by
-another characteristic.
-Defining a characteristic allows the model to track other important
-system state variables beyond the size of just one compartment.
-Examples include 'alive', 'num_inf_all', 'prop_imm', etc.
-Importantly, each compartment defined elsewhere also serves as a
-characteristic.
-Note: A code name is a representative key that developers interface
-with (e.g. in scripts and the codebase).
-It should be in lower case without spaces.</t>
         </r>
       </text>
     </comment>
@@ -254,6 +253,19 @@
         </r>
       </text>
     </comment>
+    <comment ref="G1" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <sz val="8"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>This column defines a 'default_value' attribute for a 'charac' item.</t>
+        </r>
+      </text>
+    </comment>
   </commentList>
 </comments>
 </file>
@@ -265,6 +277,28 @@
   </authors>
   <commentList>
     <comment ref="A1" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <sz val="8"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>This column is for the 'code name' of a cascade parameter.
+The base case is referred to as a transition parameter, referring to
+the flow of entities between compartments.
+However, due to the option of specifying transition rates as functions
+of other parameters, a parameter can be any variable that directly or
+indirectly affects the rate of population change in the network.
+Examples include 'b_rate', 'yes_rate', 'web_cov', etc.
+Note: A code name is a representative key that developers interface
+with (e.g. in scripts and the codebase).
+It should be in lower case without spaces.</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="B1" authorId="0">
       <text>
         <r>
           <rPr>
@@ -287,6 +321,42 @@
         </r>
       </text>
     </comment>
+    <comment ref="E1" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <sz val="8"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>This column defines a 'links' attribute for a 'par' item.</t>
+        </r>
+      </text>
+    </comment>
+  </commentList>
+</comments>
+</file>
+
+<file path=xl/comments4.xml><?xml version="1.0" encoding="utf-8"?>
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <authors>
+    <author/>
+  </authors>
+  <commentList>
+    <comment ref="A1" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <sz val="8"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>This column defines a 'name' attribute for a 'progtype' item.</t>
+        </r>
+      </text>
+    </comment>
     <comment ref="B1" authorId="0">
       <text>
         <r>
@@ -296,16 +366,33 @@
             <rFont val="Tahoma"/>
             <family val="2"/>
           </rPr>
-          <t>This column is for the 'code name' of a cascade parameter.
-The base case is referred to as a transition parameter, referring to
-the flow of entities between compartments.
-However, due to the option of specifying transition rates as functions
-of other parameters, a parameter can be any variable that directly or
-indirectly affects the rate of population change in the network.
-Examples include 'b_rate', 'yes_rate', 'web_cov', etc.
-Note: A code name is a representative key that developers interface
-with (e.g. in scripts and the codebase).
-It should be in lower case without spaces.</t>
+          <t>This column defines a 'label' attribute for a 'progtype' item.</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="C1" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <sz val="8"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>This column defines a 'name' attribute for a 'progatt' item.</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="D1" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <sz val="8"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>This column defines a 'label' attribute for a 'progatt' item.</t>
         </r>
       </text>
     </comment>
@@ -314,7 +401,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="103" uniqueCount="68">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="103" uniqueCount="69">
   <si>
     <t>Display Name</t>
   </si>
@@ -340,15 +427,6 @@
     <t>y</t>
   </si>
   <si>
-    <t>acq</t>
-  </si>
-  <si>
-    <t>screen</t>
-  </si>
-  <si>
-    <t>Function</t>
-  </si>
-  <si>
     <t>Format</t>
   </si>
   <si>
@@ -358,9 +436,6 @@
     <t>Probability</t>
   </si>
   <si>
-    <t>Average time taken to be linked to care (years)</t>
-  </si>
-  <si>
     <t>Number</t>
   </si>
   <si>
@@ -376,75 +451,6 @@
     <t>Default Value</t>
   </si>
   <si>
-    <t>death</t>
-  </si>
-  <si>
-    <t>linkage</t>
-  </si>
-  <si>
-    <t>loss</t>
-  </si>
-  <si>
-    <t>successrate</t>
-  </si>
-  <si>
-    <t>failrate</t>
-  </si>
-  <si>
-    <t>Number of people acquiring need annually</t>
-  </si>
-  <si>
-    <t>Death rate</t>
-  </si>
-  <si>
-    <t>linktime</t>
-  </si>
-  <si>
-    <t>outreach</t>
-  </si>
-  <si>
-    <t>Number covered by outreach services annually</t>
-  </si>
-  <si>
-    <t>Number of people lost to follow-up each year</t>
-  </si>
-  <si>
-    <t>Average time taken for success (years)</t>
-  </si>
-  <si>
-    <t>success_time</t>
-  </si>
-  <si>
-    <t>Probability of service failure</t>
-  </si>
-  <si>
-    <t>fail_prob</t>
-  </si>
-  <si>
-    <t>INSTRUCTIONS</t>
-  </si>
-  <si>
-    <t>Last updated:</t>
-  </si>
-  <si>
-    <t>partype</t>
-  </si>
-  <si>
-    <t>Framework file instructions</t>
-  </si>
-  <si>
-    <t>1. List the compartments in the "Compartments" sheet</t>
-  </si>
-  <si>
-    <t>2. Set up the transitions in the "Transitions" sheet</t>
-  </si>
-  <si>
-    <t>timepar</t>
-  </si>
-  <si>
-    <t>constant</t>
-  </si>
-  <si>
     <t>Susceptible</t>
   </si>
   <si>
@@ -469,18 +475,9 @@
     <t>dead</t>
   </si>
   <si>
-    <t>rec_rate</t>
-  </si>
-  <si>
     <t>foi</t>
   </si>
   <si>
-    <t>sus_death</t>
-  </si>
-  <si>
-    <t>inf_death</t>
-  </si>
-  <si>
     <t>Number ever infected</t>
   </si>
   <si>
@@ -518,6 +515,99 @@
   </si>
   <si>
     <t>sus, inf, rec</t>
+  </si>
+  <si>
+    <t>susdeath</t>
+  </si>
+  <si>
+    <t>infdeath</t>
+  </si>
+  <si>
+    <t>recrate</t>
+  </si>
+  <si>
+    <t>Par Links</t>
+  </si>
+  <si>
+    <t>Attribute Code Name</t>
+  </si>
+  <si>
+    <t>Attribute Display Name</t>
+  </si>
+  <si>
+    <t>progtype_0</t>
+  </si>
+  <si>
+    <t>Program Type 0</t>
+  </si>
+  <si>
+    <t>progtype_1</t>
+  </si>
+  <si>
+    <t>Program Type 1</t>
+  </si>
+  <si>
+    <t>progtype_2</t>
+  </si>
+  <si>
+    <t>Program Type 2</t>
+  </si>
+  <si>
+    <t>progtype_3</t>
+  </si>
+  <si>
+    <t>Program Type 3</t>
+  </si>
+  <si>
+    <t>progtype_4</t>
+  </si>
+  <si>
+    <t>Program Type 4</t>
+  </si>
+  <si>
+    <t>progtype_5</t>
+  </si>
+  <si>
+    <t>Program Type 5</t>
+  </si>
+  <si>
+    <t>progtype_6</t>
+  </si>
+  <si>
+    <t>Program Type 6</t>
+  </si>
+  <si>
+    <t>Death rate for infected people</t>
+  </si>
+  <si>
+    <t>Death rate for susceptible people</t>
+  </si>
+  <si>
+    <t>Average duration of infections (years)</t>
+  </si>
+  <si>
+    <t>contacts</t>
+  </si>
+  <si>
+    <t>Number of contacts annually</t>
+  </si>
+  <si>
+    <t>initprev</t>
+  </si>
+  <si>
+    <t>Initial prevalence</t>
+  </si>
+  <si>
+    <t>transpercontact</t>
+  </si>
+  <si>
+    <t>Transmission probability per contact</t>
+  </si>
+  <si>
+    <t>Force of infection</t>
+  </si>
+  <si>
+    <t>(1 - (1-initprev*transpercontact)**floor(contacts)*(1-initprev*transpercontact*(contacts-floor(contacts))))*(1-susdeath)</t>
   </si>
 </sst>
 </file>
@@ -529,7 +619,7 @@
     <numFmt numFmtId="164" formatCode="_-* #,##0.00_-;\-* #,##0.00_-;_-* \-??_-;_-@_-"/>
     <numFmt numFmtId="165" formatCode="_-* #,##0.00_-;\-* #,##0.00_-;_-* &quot;-&quot;??_-;_-@_-"/>
   </numFmts>
-  <fonts count="12" x14ac:knownFonts="1">
+  <fonts count="11" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -601,13 +691,6 @@
       <family val="2"/>
     </font>
     <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-    </font>
-    <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
@@ -773,7 +856,7 @@
     <xf numFmtId="9" fontId="7" fillId="0" borderId="0" applyBorder="0" applyProtection="0"/>
     <xf numFmtId="9" fontId="7" fillId="0" borderId="0" applyBorder="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -782,7 +865,6 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
@@ -796,8 +878,7 @@
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="140">
     <cellStyle name="Comma 2" xfId="9"/>
@@ -1237,169 +1318,102 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C21"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:E7"/>
   <sheetViews>
-    <sheetView zoomScale="125" workbookViewId="0">
-      <selection activeCell="C1" sqref="C1"/>
+    <sheetView zoomScale="169" zoomScaleNormal="127" workbookViewId="0">
+      <selection sqref="A1:E5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="26.5" customWidth="1"/>
-    <col min="2" max="2" width="17.1640625" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A1" s="4" t="s">
-        <v>35</v>
-      </c>
-      <c r="B1" t="s">
-        <v>36</v>
-      </c>
-      <c r="C1" s="11">
-        <f ca="1">TODAY()</f>
-        <v>43183</v>
-      </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A3" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A4" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A5" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A15" s="4"/>
-    </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A16" s="4"/>
-    </row>
-    <row r="17" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A17" s="4"/>
-    </row>
-    <row r="18" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A18" s="4"/>
-    </row>
-    <row r="19" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A19" s="4"/>
-    </row>
-    <row r="20" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A20" s="4"/>
-    </row>
-    <row r="21" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A21" s="4"/>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E7"/>
-  <sheetViews>
-    <sheetView zoomScale="169" zoomScaleNormal="127" workbookViewId="0">
-      <selection activeCell="B6" sqref="B6"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
-  <cols>
-    <col min="1" max="1" width="31.83203125" bestFit="1" customWidth="1"/>
-    <col min="2" max="5" width="15.6640625" customWidth="1"/>
+    <col min="1" max="1" width="15.6640625" customWidth="1"/>
+    <col min="2" max="2" width="31.83203125" bestFit="1" customWidth="1"/>
+    <col min="3" max="5" width="15.6640625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A1" s="1" t="s">
+      <c r="A1" s="6" t="s">
+        <v>1</v>
+      </c>
+      <c r="B1" s="6" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="C1" s="1" t="s">
+      <c r="C1" s="6" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="D1" s="6" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="E1" s="6" t="s">
         <v>4</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A2" s="2" t="s">
-        <v>43</v>
-      </c>
-      <c r="B2" s="2" t="s">
-        <v>47</v>
-      </c>
-      <c r="C2" s="2" t="s">
+      <c r="A2" s="5" t="s">
+        <v>20</v>
+      </c>
+      <c r="B2" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="C2" s="5" t="s">
         <v>7</v>
       </c>
-      <c r="D2" s="2" t="s">
+      <c r="D2" s="5" t="s">
         <v>5</v>
       </c>
-      <c r="E2" s="2" t="s">
+      <c r="E2" s="5" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A3" s="2" t="s">
-        <v>44</v>
-      </c>
-      <c r="B3" s="2" t="s">
-        <v>48</v>
-      </c>
-      <c r="C3" s="2" t="s">
+      <c r="A3" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="B3" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="C3" s="5" t="s">
         <v>5</v>
       </c>
-      <c r="D3" s="2" t="s">
+      <c r="D3" s="5" t="s">
         <v>5</v>
       </c>
-      <c r="E3" s="2" t="s">
+      <c r="E3" s="5" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A4" s="2" t="s">
-        <v>45</v>
-      </c>
-      <c r="B4" s="2" t="s">
-        <v>49</v>
-      </c>
-      <c r="C4" s="2" t="s">
+      <c r="A4" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="B4" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="C4" s="5" t="s">
         <v>5</v>
       </c>
-      <c r="D4" s="2" t="s">
+      <c r="D4" s="5" t="s">
         <v>5</v>
       </c>
-      <c r="E4" s="2" t="s">
+      <c r="E4" s="5" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A5" s="2" t="s">
-        <v>46</v>
-      </c>
-      <c r="B5" s="2" t="s">
-        <v>50</v>
-      </c>
-      <c r="C5" s="2" t="s">
+      <c r="A5" s="5" t="s">
+        <v>23</v>
+      </c>
+      <c r="B5" s="5" t="s">
+        <v>19</v>
+      </c>
+      <c r="C5" s="5" t="s">
         <v>5</v>
       </c>
-      <c r="D5" s="2" t="s">
+      <c r="D5" s="5" t="s">
         <v>7</v>
       </c>
-      <c r="E5" s="2" t="s">
+      <c r="E5" s="5" t="s">
         <v>5</v>
       </c>
     </row>
@@ -1428,12 +1442,12 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G7"/>
   <sheetViews>
     <sheetView zoomScale="171" zoomScaleNormal="224" workbookViewId="0">
-      <selection activeCell="D5" sqref="D5"/>
+      <selection activeCell="E4" sqref="E4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -1449,19 +1463,19 @@
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.2">
       <c r="B1" s="1" t="str">
-        <f>Compartments!B2</f>
+        <f>Compartments!A2</f>
         <v>sus</v>
       </c>
       <c r="C1" s="1" t="str">
-        <f>Compartments!B3</f>
+        <f>Compartments!A3</f>
         <v>inf</v>
       </c>
       <c r="D1" s="1" t="str">
-        <f>Compartments!B4</f>
+        <f>Compartments!A4</f>
         <v>rec</v>
       </c>
       <c r="E1" s="1" t="str">
-        <f>Compartments!B5</f>
+        <f>Compartments!A5</f>
         <v>dead</v>
       </c>
       <c r="F1" s="1"/>
@@ -1469,40 +1483,40 @@
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A2" s="1" t="str">
-        <f>Compartments!B2</f>
+        <f>Compartments!A2</f>
         <v>sus</v>
       </c>
       <c r="C2" t="s">
-        <v>52</v>
+        <v>24</v>
       </c>
       <c r="E2" t="s">
-        <v>53</v>
+        <v>38</v>
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A3" s="1" t="str">
-        <f>Compartments!B3</f>
+        <f>Compartments!A3</f>
         <v>inf</v>
       </c>
       <c r="D3" t="s">
-        <v>51</v>
+        <v>40</v>
       </c>
       <c r="E3" t="s">
-        <v>54</v>
+        <v>39</v>
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A4" s="1" t="str">
-        <f>Compartments!B4</f>
+        <f>Compartments!A4</f>
         <v>rec</v>
       </c>
       <c r="E4" t="s">
-        <v>53</v>
+        <v>38</v>
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A5" s="1" t="str">
-        <f>Compartments!B5</f>
+        <f>Compartments!A5</f>
         <v>dead</v>
       </c>
     </row>
@@ -1517,192 +1531,372 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F20"/>
+  <dimension ref="A1:G20"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="189" workbookViewId="0">
-      <selection activeCell="D7" sqref="D7"/>
+    <sheetView zoomScale="189" workbookViewId="0">
+      <selection activeCell="B8" sqref="B8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="28" bestFit="1" customWidth="1"/>
-    <col min="2" max="3" width="20.6640625" customWidth="1"/>
+    <col min="1" max="1" width="20.6640625" customWidth="1"/>
+    <col min="2" max="2" width="28" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="20.6640625" customWidth="1"/>
     <col min="5" max="5" width="11.1640625" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="13.33203125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="11.5" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A1" s="7" t="s">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A1" s="6" t="s">
+        <v>1</v>
+      </c>
+      <c r="B1" s="6" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="7" t="s">
-        <v>1</v>
-      </c>
-      <c r="C1" s="7" t="s">
+      <c r="C1" s="6" t="s">
         <v>6</v>
       </c>
-      <c r="D1" s="8" t="s">
-        <v>16</v>
-      </c>
-      <c r="E1" s="7" t="s">
-        <v>17</v>
-      </c>
-      <c r="F1" s="8" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A2" s="6" t="s">
-        <v>55</v>
-      </c>
-      <c r="B2" s="6" t="s">
-        <v>59</v>
-      </c>
-      <c r="C2" s="6" t="s">
-        <v>56</v>
-      </c>
-      <c r="D2" s="6"/>
-      <c r="E2" s="6"/>
-      <c r="F2" s="6"/>
-    </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A3" s="6" t="s">
-        <v>57</v>
-      </c>
-      <c r="B3" s="6" t="s">
-        <v>58</v>
-      </c>
-      <c r="C3" s="6" t="s">
-        <v>61</v>
-      </c>
-      <c r="D3" s="6"/>
-      <c r="E3" s="6"/>
-      <c r="F3" s="6"/>
-    </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A4" s="6" t="s">
-        <v>63</v>
-      </c>
-      <c r="B4" s="6" t="s">
-        <v>60</v>
-      </c>
-      <c r="C4" s="6" t="s">
-        <v>62</v>
-      </c>
-      <c r="D4" s="6"/>
-      <c r="E4" s="6"/>
-      <c r="F4" s="6"/>
-    </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A5" s="6" t="s">
-        <v>64</v>
-      </c>
-      <c r="B5" s="6" t="s">
-        <v>59</v>
-      </c>
-      <c r="C5" s="6" t="s">
-        <v>56</v>
-      </c>
-      <c r="D5" s="6"/>
-      <c r="E5" s="6" t="s">
-        <v>67</v>
-      </c>
-      <c r="F5" s="6"/>
-    </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A6" s="6" t="s">
-        <v>65</v>
-      </c>
-      <c r="B6" s="6" t="s">
-        <v>58</v>
-      </c>
-      <c r="C6" s="6" t="s">
-        <v>61</v>
-      </c>
-      <c r="D6" s="6"/>
-      <c r="E6" s="6" t="s">
-        <v>67</v>
-      </c>
-      <c r="F6" s="6"/>
-    </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A7" s="6" t="s">
-        <v>66</v>
-      </c>
-      <c r="B7" s="6" t="s">
-        <v>60</v>
-      </c>
-      <c r="C7" s="6" t="s">
-        <v>62</v>
-      </c>
-      <c r="D7" s="6"/>
-      <c r="E7" s="6" t="s">
-        <v>67</v>
-      </c>
-      <c r="F7" s="6"/>
-    </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A8" s="6"/>
-      <c r="B8" s="6"/>
-      <c r="C8" s="6"/>
-      <c r="D8" s="6"/>
-      <c r="E8" s="6"/>
-      <c r="F8" s="6"/>
-    </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A9" s="6"/>
-      <c r="B9" s="6"/>
-      <c r="C9" s="6"/>
-      <c r="D9" s="6"/>
-      <c r="E9" s="6"/>
-      <c r="F9" s="6"/>
-    </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="D1" s="7" t="s">
+        <v>12</v>
+      </c>
+      <c r="E1" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="F1" s="7" t="s">
+        <v>14</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A2" s="5" t="s">
+        <v>29</v>
+      </c>
+      <c r="B2" s="5" t="s">
+        <v>25</v>
+      </c>
+      <c r="C2" s="5" t="s">
+        <v>26</v>
+      </c>
+      <c r="D2" s="5"/>
+      <c r="E2" s="5"/>
+      <c r="F2" s="5"/>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A3" s="5" t="s">
+        <v>28</v>
+      </c>
+      <c r="B3" s="5" t="s">
+        <v>27</v>
+      </c>
+      <c r="C3" s="5" t="s">
+        <v>31</v>
+      </c>
+      <c r="D3" s="5"/>
+      <c r="E3" s="5"/>
+      <c r="F3" s="5"/>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A4" s="5" t="s">
+        <v>30</v>
+      </c>
+      <c r="B4" s="5" t="s">
+        <v>33</v>
+      </c>
+      <c r="C4" s="5" t="s">
+        <v>32</v>
+      </c>
+      <c r="D4" s="5"/>
+      <c r="E4" s="5"/>
+      <c r="F4" s="5"/>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A5" s="5" t="s">
+        <v>29</v>
+      </c>
+      <c r="B5" s="5" t="s">
+        <v>34</v>
+      </c>
+      <c r="C5" s="5" t="s">
+        <v>26</v>
+      </c>
+      <c r="D5" s="5"/>
+      <c r="E5" s="5" t="s">
+        <v>37</v>
+      </c>
+      <c r="F5" s="5"/>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A6" s="5" t="s">
+        <v>28</v>
+      </c>
+      <c r="B6" s="5" t="s">
+        <v>35</v>
+      </c>
+      <c r="C6" s="5" t="s">
+        <v>31</v>
+      </c>
+      <c r="D6" s="5"/>
+      <c r="E6" s="5" t="s">
+        <v>37</v>
+      </c>
+      <c r="F6" s="5"/>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A7" s="5" t="s">
+        <v>30</v>
+      </c>
+      <c r="B7" s="5" t="s">
+        <v>36</v>
+      </c>
+      <c r="C7" s="5" t="s">
+        <v>32</v>
+      </c>
+      <c r="D7" s="5"/>
+      <c r="E7" s="5" t="s">
+        <v>37</v>
+      </c>
+      <c r="F7" s="5"/>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A8" s="5"/>
+      <c r="B8" s="5"/>
+      <c r="C8" s="5"/>
+      <c r="D8" s="5"/>
+      <c r="E8" s="5"/>
+      <c r="F8" s="5"/>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A9" s="5"/>
+      <c r="B9" s="5"/>
+      <c r="C9" s="5"/>
+      <c r="D9" s="5"/>
+      <c r="E9" s="5"/>
+      <c r="F9" s="5"/>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A10" s="2"/>
       <c r="B10" s="2"/>
       <c r="C10" s="2"/>
       <c r="E10" s="2"/>
     </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A11" s="2"/>
       <c r="B11" s="2"/>
       <c r="C11" s="2"/>
       <c r="D11" s="2"/>
       <c r="E11" s="2"/>
     </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A12" s="2"/>
       <c r="B12" s="2"/>
       <c r="C12" s="2"/>
       <c r="D12" s="2"/>
       <c r="E12" s="2"/>
     </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A13" s="2"/>
       <c r="B13" s="2"/>
       <c r="C13" s="2"/>
       <c r="D13" s="2"/>
       <c r="E13" s="2"/>
     </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="B15" s="2"/>
+    </row>
+    <row r="16" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="B16" s="2"/>
+    </row>
+    <row r="17" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B17" s="2"/>
+    </row>
+    <row r="18" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B18" s="2"/>
+    </row>
+    <row r="19" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B19" s="2"/>
+    </row>
+    <row r="20" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B20" s="2"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <legacyDrawing r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:E16"/>
+  <sheetViews>
+    <sheetView tabSelected="1" zoomScale="160" workbookViewId="0">
+      <selection activeCell="C6" sqref="C6"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="11.1640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="36.6640625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="9.1640625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="11.6640625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A1" s="6" t="s">
+        <v>1</v>
+      </c>
+      <c r="B1" s="6" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" s="7" t="s">
+        <v>8</v>
+      </c>
+      <c r="D1" s="7" t="s">
+        <v>15</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A2" s="5" t="s">
+        <v>63</v>
+      </c>
+      <c r="B2" s="4" t="s">
+        <v>64</v>
+      </c>
+      <c r="C2" t="s">
+        <v>10</v>
+      </c>
+      <c r="D2" s="9">
+        <v>5.0000000000000001E-3</v>
+      </c>
+      <c r="E2" s="8"/>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A3" s="5" t="s">
+        <v>65</v>
+      </c>
+      <c r="B3" s="4" t="s">
+        <v>66</v>
+      </c>
+      <c r="C3" t="s">
+        <v>10</v>
+      </c>
+      <c r="D3" s="9">
+        <v>8.0000000000000004E-4</v>
+      </c>
+      <c r="E3" s="8"/>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A4" s="5" t="s">
+        <v>61</v>
+      </c>
+      <c r="B4" s="4" t="s">
+        <v>62</v>
+      </c>
+      <c r="C4" t="s">
+        <v>11</v>
+      </c>
+      <c r="D4">
+        <v>80</v>
+      </c>
+      <c r="E4" s="8"/>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A5" s="5" t="s">
+        <v>24</v>
+      </c>
+      <c r="B5" s="4" t="s">
+        <v>67</v>
+      </c>
+      <c r="C5" t="s">
+        <v>10</v>
+      </c>
+      <c r="E5" s="8" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A6" s="5" t="s">
+        <v>40</v>
+      </c>
+      <c r="B6" s="4" t="s">
+        <v>60</v>
+      </c>
+      <c r="C6" t="s">
+        <v>9</v>
+      </c>
+      <c r="D6">
+        <v>0.5</v>
+      </c>
+      <c r="E6" s="8"/>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A7" s="5" t="s">
+        <v>39</v>
+      </c>
+      <c r="B7" s="4" t="s">
+        <v>58</v>
+      </c>
+      <c r="C7" t="s">
+        <v>10</v>
+      </c>
+      <c r="D7" s="3">
+        <v>1.6E-2</v>
+      </c>
+      <c r="E7" s="8"/>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A8" s="5" t="s">
+        <v>38</v>
+      </c>
+      <c r="B8" s="4" t="s">
+        <v>59</v>
+      </c>
+      <c r="C8" t="s">
+        <v>10</v>
+      </c>
+      <c r="D8" s="3">
+        <v>8.0000000000000002E-3</v>
+      </c>
+      <c r="E8" s="8"/>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A9" s="2"/>
+      <c r="B9" s="2"/>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A10" s="2"/>
+      <c r="B10" s="2"/>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A11" s="2"/>
+      <c r="B11" s="2"/>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A12" s="2"/>
+      <c r="B12" s="2"/>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A13" s="2"/>
+      <c r="B13" s="2"/>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A14" s="2"/>
+      <c r="B14" s="2"/>
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A15" s="2"/>
-    </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="B15" s="2"/>
+    </row>
+    <row r="16" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A16" s="2"/>
-    </row>
-    <row r="17" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A17" s="2"/>
-    </row>
-    <row r="18" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A18" s="2"/>
-    </row>
-    <row r="19" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A19" s="2"/>
-    </row>
-    <row r="20" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A20" s="2"/>
+      <c r="B16" s="2"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -1712,212 +1906,282 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H16"/>
+  <dimension ref="A1:D22"/>
   <sheetViews>
-    <sheetView zoomScale="160" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:D22"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
-  <cols>
-    <col min="1" max="1" width="36.6640625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="11.1640625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="7.83203125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="9.1640625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="11.6640625" bestFit="1" customWidth="1"/>
-  </cols>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A1" s="7" t="s">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="B1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="7" t="s">
-        <v>1</v>
-      </c>
-      <c r="C1" s="8" t="s">
-        <v>10</v>
-      </c>
-      <c r="D1" s="8" t="s">
-        <v>11</v>
-      </c>
-      <c r="E1" s="8" t="s">
-        <v>19</v>
-      </c>
-      <c r="F1" s="9" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A2" s="5" t="s">
-        <v>25</v>
-      </c>
-      <c r="B2" s="6" t="s">
-        <v>8</v>
-      </c>
-      <c r="D2" t="s">
-        <v>15</v>
-      </c>
-      <c r="E2">
-        <v>100</v>
-      </c>
-      <c r="F2" s="10" t="s">
-        <v>41</v>
-      </c>
-      <c r="H2" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A3" s="5" t="s">
-        <v>29</v>
-      </c>
-      <c r="B3" s="6" t="s">
-        <v>9</v>
-      </c>
-      <c r="D3" t="s">
-        <v>13</v>
-      </c>
-      <c r="F3" s="10" t="s">
-        <v>41</v>
-      </c>
-      <c r="H3" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A4" s="5" t="s">
-        <v>14</v>
-      </c>
-      <c r="B4" s="6" t="s">
-        <v>27</v>
-      </c>
-      <c r="D4" t="s">
-        <v>12</v>
-      </c>
-      <c r="F4" s="10" t="s">
-        <v>41</v>
-      </c>
-      <c r="H4" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A5" s="5" t="s">
-        <v>30</v>
-      </c>
-      <c r="B5" s="6" t="s">
-        <v>22</v>
-      </c>
-      <c r="D5" t="s">
-        <v>15</v>
-      </c>
-      <c r="F5" s="10" t="s">
-        <v>41</v>
-      </c>
-      <c r="H5" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A6" s="5" t="s">
-        <v>31</v>
-      </c>
-      <c r="B6" s="6" t="s">
-        <v>32</v>
-      </c>
-      <c r="D6" t="s">
-        <v>12</v>
-      </c>
-      <c r="F6" s="10" t="s">
+      <c r="C1" s="1" t="s">
         <v>42</v>
       </c>
-      <c r="H6" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A7" s="5" t="s">
-        <v>33</v>
-      </c>
-      <c r="B7" s="6" t="s">
-        <v>34</v>
-      </c>
-      <c r="D7" t="s">
-        <v>13</v>
-      </c>
-      <c r="F7" s="10" t="s">
-        <v>42</v>
-      </c>
-      <c r="H7" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A8" s="5" t="s">
-        <v>26</v>
-      </c>
-      <c r="B8" s="6" t="s">
-        <v>20</v>
-      </c>
-      <c r="D8" t="s">
-        <v>13</v>
-      </c>
-      <c r="E8" s="3">
-        <v>0.02</v>
-      </c>
-      <c r="F8" s="10" t="s">
-        <v>42</v>
-      </c>
-      <c r="H8" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A9" s="2"/>
-      <c r="B9" s="2"/>
-    </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A10" s="2"/>
-      <c r="B10" s="2"/>
-    </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A11" s="2"/>
-      <c r="B11" s="2"/>
-    </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A12" s="2"/>
-      <c r="B12" s="2"/>
-    </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A13" s="2"/>
-      <c r="B13" s="2"/>
-    </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A14" s="2"/>
-      <c r="B14" s="2"/>
-    </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A15" s="2"/>
-      <c r="B15" s="2"/>
-    </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A16" s="2"/>
-      <c r="B16" s="2"/>
+      <c r="D1" s="1" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A2" s="2" t="s">
+        <v>44</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="C2" s="2" t="str">
+        <f>CONCATENATE(A2,"_att_0")</f>
+        <v>progtype_0_att_0</v>
+      </c>
+      <c r="D2" s="2" t="str">
+        <f>CONCATENATE(B2," - Attribute 0")</f>
+        <v>Program Type 0 - Attribute 0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="C3" s="2" t="str">
+        <f>CONCATENATE(A2,"_att_1")</f>
+        <v>progtype_0_att_1</v>
+      </c>
+      <c r="D3" s="2" t="str">
+        <f>CONCATENATE(B2," - Attribute 1")</f>
+        <v>Program Type 0 - Attribute 1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="C4" s="2" t="str">
+        <f>CONCATENATE(A2,"_att_2")</f>
+        <v>progtype_0_att_2</v>
+      </c>
+      <c r="D4" s="2" t="str">
+        <f>CONCATENATE(B2," - Attribute 2")</f>
+        <v>Program Type 0 - Attribute 2</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A5" s="2" t="s">
+        <v>46</v>
+      </c>
+      <c r="B5" s="2" t="s">
+        <v>47</v>
+      </c>
+      <c r="C5" s="2" t="str">
+        <f>CONCATENATE(A5,"_att_0")</f>
+        <v>progtype_1_att_0</v>
+      </c>
+      <c r="D5" s="2" t="str">
+        <f>CONCATENATE(B5," - Attribute 0")</f>
+        <v>Program Type 1 - Attribute 0</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="C6" s="2" t="str">
+        <f>CONCATENATE(A5,"_att_1")</f>
+        <v>progtype_1_att_1</v>
+      </c>
+      <c r="D6" s="2" t="str">
+        <f>CONCATENATE(B5," - Attribute 1")</f>
+        <v>Program Type 1 - Attribute 1</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="C7" s="2" t="str">
+        <f>CONCATENATE(A5,"_att_2")</f>
+        <v>progtype_1_att_2</v>
+      </c>
+      <c r="D7" s="2" t="str">
+        <f>CONCATENATE(B5," - Attribute 2")</f>
+        <v>Program Type 1 - Attribute 2</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A8" s="2" t="s">
+        <v>48</v>
+      </c>
+      <c r="B8" s="2" t="s">
+        <v>49</v>
+      </c>
+      <c r="C8" s="2" t="str">
+        <f>CONCATENATE(A8,"_att_0")</f>
+        <v>progtype_2_att_0</v>
+      </c>
+      <c r="D8" s="2" t="str">
+        <f>CONCATENATE(B8," - Attribute 0")</f>
+        <v>Program Type 2 - Attribute 0</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="C9" s="2" t="str">
+        <f>CONCATENATE(A8,"_att_1")</f>
+        <v>progtype_2_att_1</v>
+      </c>
+      <c r="D9" s="2" t="str">
+        <f>CONCATENATE(B8," - Attribute 1")</f>
+        <v>Program Type 2 - Attribute 1</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="C10" s="2" t="str">
+        <f>CONCATENATE(A8,"_att_2")</f>
+        <v>progtype_2_att_2</v>
+      </c>
+      <c r="D10" s="2" t="str">
+        <f>CONCATENATE(B8," - Attribute 2")</f>
+        <v>Program Type 2 - Attribute 2</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A11" s="2" t="s">
+        <v>50</v>
+      </c>
+      <c r="B11" s="2" t="s">
+        <v>51</v>
+      </c>
+      <c r="C11" s="2" t="str">
+        <f>CONCATENATE(A11,"_att_0")</f>
+        <v>progtype_3_att_0</v>
+      </c>
+      <c r="D11" s="2" t="str">
+        <f>CONCATENATE(B11," - Attribute 0")</f>
+        <v>Program Type 3 - Attribute 0</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="C12" s="2" t="str">
+        <f>CONCATENATE(A11,"_att_1")</f>
+        <v>progtype_3_att_1</v>
+      </c>
+      <c r="D12" s="2" t="str">
+        <f>CONCATENATE(B11," - Attribute 1")</f>
+        <v>Program Type 3 - Attribute 1</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="C13" s="2" t="str">
+        <f>CONCATENATE(A11,"_att_2")</f>
+        <v>progtype_3_att_2</v>
+      </c>
+      <c r="D13" s="2" t="str">
+        <f>CONCATENATE(B11," - Attribute 2")</f>
+        <v>Program Type 3 - Attribute 2</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A14" s="2" t="s">
+        <v>52</v>
+      </c>
+      <c r="B14" s="2" t="s">
+        <v>53</v>
+      </c>
+      <c r="C14" s="2" t="str">
+        <f>CONCATENATE(A14,"_att_0")</f>
+        <v>progtype_4_att_0</v>
+      </c>
+      <c r="D14" s="2" t="str">
+        <f>CONCATENATE(B14," - Attribute 0")</f>
+        <v>Program Type 4 - Attribute 0</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="C15" s="2" t="str">
+        <f>CONCATENATE(A14,"_att_1")</f>
+        <v>progtype_4_att_1</v>
+      </c>
+      <c r="D15" s="2" t="str">
+        <f>CONCATENATE(B14," - Attribute 1")</f>
+        <v>Program Type 4 - Attribute 1</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="C16" s="2" t="str">
+        <f>CONCATENATE(A14,"_att_2")</f>
+        <v>progtype_4_att_2</v>
+      </c>
+      <c r="D16" s="2" t="str">
+        <f>CONCATENATE(B14," - Attribute 2")</f>
+        <v>Program Type 4 - Attribute 2</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A17" s="2" t="s">
+        <v>54</v>
+      </c>
+      <c r="B17" s="2" t="s">
+        <v>55</v>
+      </c>
+      <c r="C17" s="2" t="str">
+        <f>CONCATENATE(A17,"_att_0")</f>
+        <v>progtype_5_att_0</v>
+      </c>
+      <c r="D17" s="2" t="str">
+        <f>CONCATENATE(B17," - Attribute 0")</f>
+        <v>Program Type 5 - Attribute 0</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="C18" s="2" t="str">
+        <f>CONCATENATE(A17,"_att_1")</f>
+        <v>progtype_5_att_1</v>
+      </c>
+      <c r="D18" s="2" t="str">
+        <f>CONCATENATE(B17," - Attribute 1")</f>
+        <v>Program Type 5 - Attribute 1</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="C19" s="2" t="str">
+        <f>CONCATENATE(A17,"_att_2")</f>
+        <v>progtype_5_att_2</v>
+      </c>
+      <c r="D19" s="2" t="str">
+        <f>CONCATENATE(B17," - Attribute 2")</f>
+        <v>Program Type 5 - Attribute 2</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A20" s="2" t="s">
+        <v>56</v>
+      </c>
+      <c r="B20" s="2" t="s">
+        <v>57</v>
+      </c>
+      <c r="C20" s="2" t="str">
+        <f>CONCATENATE(A20,"_att_0")</f>
+        <v>progtype_6_att_0</v>
+      </c>
+      <c r="D20" s="2" t="str">
+        <f>CONCATENATE(B20," - Attribute 0")</f>
+        <v>Program Type 6 - Attribute 0</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="C21" s="2" t="str">
+        <f>CONCATENATE(A20,"_att_1")</f>
+        <v>progtype_6_att_1</v>
+      </c>
+      <c r="D21" s="2" t="str">
+        <f>CONCATENATE(B20," - Attribute 1")</f>
+        <v>Program Type 6 - Attribute 1</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="C22" s="2" t="str">
+        <f>CONCATENATE(A20,"_att_2")</f>
+        <v>progtype_6_att_2</v>
+      </c>
+      <c r="D22" s="2" t="str">
+        <f>CONCATENATE(B20," - Attribute 2")</f>
+        <v>Program Type 6 - Attribute 2</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <legacyDrawing r:id="rId1"/>
 </worksheet>
-</file>
-
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
-  <sheetData/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
 </file>
</xml_diff>

<commit_message>
Update frameworks files for impact tags
This commit updates parameter sheets with a column to mark impact parameters, but it is not clear yet how to set up program impacts for either test case.
</commit_message>
<xml_diff>
--- a/tests/frameworks/framework_sir.xlsx
+++ b/tests/frameworks/framework_sir.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="19126"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="19226"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Projects - Work\Optima\atomica\tests\frameworks\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F4A949E8-73A3-4F97-B7FB-DFCFC73DE8CE}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D5F5411F-FE0D-47CA-BD25-7CEBFD11B4F1}" xr6:coauthVersionLast="32" xr6:coauthVersionMax="32" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="240" yWindow="15" windowWidth="16095" windowHeight="9660" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -17,7 +17,6 @@
     <sheet name="Transitions" sheetId="2" r:id="rId2"/>
     <sheet name="Characteristics" sheetId="3" r:id="rId3"/>
     <sheet name="Parameters" sheetId="4" r:id="rId4"/>
-    <sheet name="Program Types" sheetId="5" r:id="rId5"/>
   </sheets>
   <calcPr calcId="179017"/>
 </workbook>
@@ -426,7 +425,29 @@
         </r>
       </text>
     </comment>
-    <comment ref="D1" authorId="0" shapeId="0" xr:uid="{65E32CD1-EF29-4034-8FD9-2B2CA808AD0D}">
+    <comment ref="D1" authorId="0" shapeId="0" xr:uid="{AA874E47-9695-4A49-BCCA-66E5B118006C}">
+      <text>
+        <r>
+          <rPr>
+            <sz val="8"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>This column is for tagging a parameter as an impact, which means
+that programs can map a budget to a value for this parameter.
+Currently, the user will choose which programs impact this
+parameter within a databook constructed from this framework file.
+Notably, if this tag is active, the parameter cannot be expressed
+as a function of other parameters as its value will be directly
+overwritten if programs are active.
+Note: This tag is only enabled for a parameter by marking the
+corresponding cell 'y'.
+Anything else, including keeping the cell blank, disables the tag.</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="E1" authorId="0" shapeId="0" xr:uid="{65E32CD1-EF29-4034-8FD9-2B2CA808AD0D}">
       <text>
         <r>
           <rPr>
@@ -439,7 +460,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="E1" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0300-000004000000}">
+    <comment ref="F1" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0300-000004000000}">
       <text>
         <r>
           <rPr>
@@ -452,7 +473,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="F1" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0300-000005000000}">
+    <comment ref="G1" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0300-000005000000}">
       <text>
         <r>
           <rPr>
@@ -462,68 +483,6 @@
             <family val="2"/>
           </rPr>
           <t>This column defines a 'function' attribute for a 'par' item.</t>
-        </r>
-      </text>
-    </comment>
-  </commentList>
-</comments>
-</file>
-
-<file path=xl/comments4.xml><?xml version="1.0" encoding="utf-8"?>
-<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
-  <authors>
-    <author/>
-  </authors>
-  <commentList>
-    <comment ref="A1" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0400-000001000000}">
-      <text>
-        <r>
-          <rPr>
-            <sz val="8"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t>This column defines a 'name' attribute for a 'progtype' item.</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="B1" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0400-000002000000}">
-      <text>
-        <r>
-          <rPr>
-            <sz val="8"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t>This column defines a 'label' attribute for a 'progtype' item.</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="C1" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0400-000003000000}">
-      <text>
-        <r>
-          <rPr>
-            <sz val="8"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t>This column defines a 'name' attribute for a 'progatt' item.</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="D1" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0400-000004000000}">
-      <text>
-        <r>
-          <rPr>
-            <sz val="8"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t>This column defines a 'label' attribute for a 'progatt' item.</t>
         </r>
       </text>
     </comment>
@@ -532,7 +491,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="110" uniqueCount="74">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="99" uniqueCount="59">
   <si>
     <t>Code Name</t>
   </si>
@@ -570,54 +529,6 @@
     <t>Function</t>
   </si>
   <si>
-    <t>Attribute Code Name</t>
-  </si>
-  <si>
-    <t>Attribute Display Name</t>
-  </si>
-  <si>
-    <t>progtype_0</t>
-  </si>
-  <si>
-    <t>Program Type 0</t>
-  </si>
-  <si>
-    <t>progtype_1</t>
-  </si>
-  <si>
-    <t>Program Type 1</t>
-  </si>
-  <si>
-    <t>progtype_2</t>
-  </si>
-  <si>
-    <t>Program Type 2</t>
-  </si>
-  <si>
-    <t>progtype_3</t>
-  </si>
-  <si>
-    <t>Program Type 3</t>
-  </si>
-  <si>
-    <t>progtype_4</t>
-  </si>
-  <si>
-    <t>Program Type 4</t>
-  </si>
-  <si>
-    <t>progtype_5</t>
-  </si>
-  <si>
-    <t>Program Type 5</t>
-  </si>
-  <si>
-    <t>progtype_6</t>
-  </si>
-  <si>
-    <t>Program Type 6</t>
-  </si>
-  <si>
     <t>sus</t>
   </si>
   <si>
@@ -754,6 +665,9 @@
   </si>
   <si>
     <t>(1 - (1-ch_prev*transpercontact)**floor(contacts)*(1-ch_prev*transpercontact*(contacts-floor(contacts))))*(1-susdeath)</t>
+  </si>
+  <si>
+    <t>Is Impact</t>
   </si>
 </sst>
 </file>
@@ -1199,15 +1113,15 @@
         <v>8</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>70</v>
+        <v>54</v>
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A2" s="3" t="s">
-        <v>28</v>
+        <v>12</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>29</v>
+        <v>13</v>
       </c>
       <c r="C2" s="3" t="s">
         <v>5</v>
@@ -1225,10 +1139,10 @@
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A3" s="3" t="s">
-        <v>30</v>
+        <v>14</v>
       </c>
       <c r="B3" s="3" t="s">
-        <v>31</v>
+        <v>15</v>
       </c>
       <c r="C3" s="3" t="s">
         <v>5</v>
@@ -1248,10 +1162,10 @@
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A4" s="3" t="s">
-        <v>32</v>
+        <v>16</v>
       </c>
       <c r="B4" s="3" t="s">
-        <v>33</v>
+        <v>17</v>
       </c>
       <c r="C4" s="3" t="s">
         <v>5</v>
@@ -1271,16 +1185,16 @@
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A5" s="3" t="s">
-        <v>34</v>
+        <v>18</v>
       </c>
       <c r="B5" s="3" t="s">
-        <v>35</v>
+        <v>19</v>
       </c>
       <c r="C5" s="3" t="s">
         <v>5</v>
       </c>
       <c r="D5" s="3" t="s">
-        <v>36</v>
+        <v>20</v>
       </c>
       <c r="E5" s="3" t="s">
         <v>5</v>
@@ -1340,10 +1254,10 @@
         <v>sus</v>
       </c>
       <c r="C2" t="s">
-        <v>37</v>
+        <v>21</v>
       </c>
       <c r="E2" t="s">
-        <v>38</v>
+        <v>22</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.45">
@@ -1352,10 +1266,10 @@
         <v>inf</v>
       </c>
       <c r="D3" t="s">
-        <v>39</v>
+        <v>23</v>
       </c>
       <c r="E3" t="s">
-        <v>40</v>
+        <v>24</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.45">
@@ -1364,7 +1278,7 @@
         <v>rec</v>
       </c>
       <c r="E4" t="s">
-        <v>38</v>
+        <v>22</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.45">
@@ -1407,7 +1321,7 @@
         <v>8</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>70</v>
+        <v>54</v>
       </c>
       <c r="E1" s="1" t="s">
         <v>6</v>
@@ -1421,46 +1335,46 @@
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A2" s="4" t="s">
-        <v>41</v>
+        <v>25</v>
       </c>
       <c r="B2" s="4" t="s">
-        <v>42</v>
+        <v>26</v>
       </c>
       <c r="C2" s="2"/>
       <c r="D2" s="2">
         <v>1</v>
       </c>
       <c r="E2" s="3" t="s">
-        <v>43</v>
+        <v>27</v>
       </c>
       <c r="F2" s="4"/>
       <c r="G2" s="2"/>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A3" s="4" t="s">
-        <v>71</v>
+        <v>55</v>
       </c>
       <c r="B3" s="4" t="s">
-        <v>72</v>
+        <v>56</v>
       </c>
       <c r="C3" s="2"/>
       <c r="D3" s="2">
         <v>1</v>
       </c>
       <c r="E3" s="3" t="s">
-        <v>30</v>
+        <v>14</v>
       </c>
       <c r="F3" s="4" t="s">
-        <v>41</v>
+        <v>25</v>
       </c>
       <c r="G3" s="2"/>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A4" s="3" t="s">
-        <v>44</v>
+        <v>28</v>
       </c>
       <c r="B4" s="3" t="s">
-        <v>45</v>
+        <v>29</v>
       </c>
       <c r="C4" s="2">
         <v>-1</v>
@@ -1469,17 +1383,17 @@
         <v>1</v>
       </c>
       <c r="E4" s="3" t="s">
-        <v>46</v>
+        <v>30</v>
       </c>
       <c r="F4" s="3"/>
       <c r="G4" s="2"/>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A5" s="3" t="s">
-        <v>47</v>
+        <v>31</v>
       </c>
       <c r="B5" s="3" t="s">
-        <v>48</v>
+        <v>32</v>
       </c>
       <c r="C5" s="2">
         <v>-1</v>
@@ -1488,17 +1402,17 @@
         <v>1</v>
       </c>
       <c r="E5" s="3" t="s">
-        <v>49</v>
+        <v>33</v>
       </c>
       <c r="F5" s="3"/>
       <c r="G5" s="2"/>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A6" s="3" t="s">
-        <v>50</v>
+        <v>34</v>
       </c>
       <c r="B6" s="3" t="s">
-        <v>57</v>
+        <v>41</v>
       </c>
       <c r="C6" s="2">
         <v>-1</v>
@@ -1507,17 +1421,17 @@
         <v>1</v>
       </c>
       <c r="E6" s="3" t="s">
-        <v>51</v>
+        <v>35</v>
       </c>
       <c r="F6" s="3"/>
       <c r="G6" s="2"/>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A7" s="3" t="s">
-        <v>52</v>
+        <v>36</v>
       </c>
       <c r="B7" s="3" t="s">
-        <v>53</v>
+        <v>37</v>
       </c>
       <c r="C7" s="2">
         <v>-1</v>
@@ -1526,19 +1440,19 @@
         <v>1</v>
       </c>
       <c r="E7" s="3" t="s">
-        <v>44</v>
+        <v>28</v>
       </c>
       <c r="F7" s="3" t="s">
-        <v>41</v>
+        <v>25</v>
       </c>
       <c r="G7" s="2"/>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A8" s="3" t="s">
-        <v>54</v>
+        <v>38</v>
       </c>
       <c r="B8" s="3" t="s">
-        <v>55</v>
+        <v>39</v>
       </c>
       <c r="C8" s="2">
         <v>-1</v>
@@ -1547,19 +1461,19 @@
         <v>1</v>
       </c>
       <c r="E8" s="3" t="s">
-        <v>47</v>
+        <v>31</v>
       </c>
       <c r="F8" s="3" t="s">
-        <v>41</v>
+        <v>25</v>
       </c>
       <c r="G8" s="2"/>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A9" s="3" t="s">
-        <v>56</v>
+        <v>40</v>
       </c>
       <c r="B9" s="3" t="s">
-        <v>58</v>
+        <v>42</v>
       </c>
       <c r="C9" s="2">
         <v>-1</v>
@@ -1568,10 +1482,10 @@
         <v>1</v>
       </c>
       <c r="E9" s="3" t="s">
-        <v>50</v>
+        <v>34</v>
       </c>
       <c r="F9" s="3" t="s">
-        <v>41</v>
+        <v>25</v>
       </c>
       <c r="G9" s="2"/>
     </row>
@@ -1583,10 +1497,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
-  <dimension ref="A1:F7"/>
+  <dimension ref="A1:G7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:XFD2"/>
+      <selection activeCell="E12" sqref="E12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -1594,12 +1508,13 @@
     <col min="1" max="1" width="13.265625" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="30.6640625" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="9.265625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="13.86328125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="11.73046875" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="96.33203125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="8.1328125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="13.86328125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="11.73046875" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="96.33203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1610,397 +1525,139 @@
         <v>10</v>
       </c>
       <c r="D1" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="E1" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="F1" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="G1" s="1" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A2" s="3" t="s">
-        <v>60</v>
+        <v>44</v>
       </c>
       <c r="B2" s="5" t="s">
-        <v>61</v>
+        <v>45</v>
       </c>
       <c r="C2" t="s">
-        <v>59</v>
-      </c>
-      <c r="D2" s="2"/>
-      <c r="E2" s="6">
+        <v>43</v>
+      </c>
+      <c r="D2" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="E2" s="2"/>
+      <c r="F2" s="6">
         <v>8.0000000000000004E-4</v>
       </c>
-      <c r="F2" s="7"/>
-    </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="G2" s="7"/>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A3" s="3" t="s">
-        <v>62</v>
+        <v>46</v>
       </c>
       <c r="B3" s="5" t="s">
-        <v>63</v>
+        <v>47</v>
       </c>
       <c r="C3" t="s">
-        <v>64</v>
-      </c>
-      <c r="D3" s="2"/>
-      <c r="E3">
+        <v>48</v>
+      </c>
+      <c r="D3" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="E3" s="2"/>
+      <c r="F3">
         <v>80</v>
       </c>
-      <c r="F3" s="7"/>
-    </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="G3" s="7"/>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A4" s="3" t="s">
-        <v>37</v>
+        <v>21</v>
       </c>
       <c r="B4" s="5" t="s">
-        <v>65</v>
+        <v>49</v>
       </c>
       <c r="C4" t="s">
-        <v>59</v>
-      </c>
-      <c r="D4" s="2">
+        <v>43</v>
+      </c>
+      <c r="D4" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="E4" s="2">
         <v>-1</v>
       </c>
-      <c r="F4" s="7" t="s">
-        <v>73</v>
-      </c>
-    </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="G4" s="7" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A5" s="3" t="s">
-        <v>39</v>
+        <v>23</v>
       </c>
       <c r="B5" s="5" t="s">
-        <v>66</v>
+        <v>50</v>
       </c>
       <c r="C5" t="s">
-        <v>67</v>
-      </c>
-      <c r="D5" s="2"/>
-      <c r="E5">
+        <v>51</v>
+      </c>
+      <c r="D5" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="E5" s="2"/>
+      <c r="F5">
         <v>0.5</v>
       </c>
-      <c r="F5" s="7"/>
-    </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="G5" s="7"/>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A6" s="3" t="s">
-        <v>40</v>
+        <v>24</v>
       </c>
       <c r="B6" s="5" t="s">
-        <v>68</v>
+        <v>52</v>
       </c>
       <c r="C6" t="s">
-        <v>59</v>
-      </c>
-      <c r="D6" s="2"/>
-      <c r="E6" s="8">
+        <v>43</v>
+      </c>
+      <c r="D6" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="E6" s="2"/>
+      <c r="F6" s="8">
         <v>1.6E-2</v>
       </c>
-      <c r="F6" s="7"/>
-    </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="G6" s="7"/>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A7" s="3" t="s">
-        <v>38</v>
+        <v>22</v>
       </c>
       <c r="B7" s="5" t="s">
-        <v>69</v>
+        <v>53</v>
       </c>
       <c r="C7" t="s">
-        <v>59</v>
-      </c>
-      <c r="D7" s="2"/>
-      <c r="E7" s="8">
+        <v>43</v>
+      </c>
+      <c r="D7" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="E7" s="2"/>
+      <c r="F7" s="8">
         <v>8.0000000000000002E-3</v>
       </c>
-      <c r="F7" s="7"/>
+      <c r="G7" s="7"/>
     </row>
   </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <legacyDrawing r:id="rId1"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
-  <dimension ref="A1:D22"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
-  <cols>
-    <col min="1" max="3" width="20.73046875" customWidth="1"/>
-    <col min="4" max="4" width="25.73046875" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.45">
-      <c r="A1" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.45">
-      <c r="A2" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="B2" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="C2" s="2" t="str">
-        <f>CONCATENATE(A2,"_att_0")</f>
-        <v>progtype_0_att_0</v>
-      </c>
-      <c r="D2" s="2" t="str">
-        <f>CONCATENATE(B2," - Attribute 0")</f>
-        <v>Program Type 0 - Attribute 0</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.45">
-      <c r="C3" s="2" t="str">
-        <f>CONCATENATE(A2,"_att_1")</f>
-        <v>progtype_0_att_1</v>
-      </c>
-      <c r="D3" s="2" t="str">
-        <f>CONCATENATE(B2," - Attribute 1")</f>
-        <v>Program Type 0 - Attribute 1</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.45">
-      <c r="C4" s="2" t="str">
-        <f>CONCATENATE(A2,"_att_2")</f>
-        <v>progtype_0_att_2</v>
-      </c>
-      <c r="D4" s="2" t="str">
-        <f>CONCATENATE(B2," - Attribute 2")</f>
-        <v>Program Type 0 - Attribute 2</v>
-      </c>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.45">
-      <c r="A5" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="B5" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="C5" s="2" t="str">
-        <f>CONCATENATE(A5,"_att_0")</f>
-        <v>progtype_1_att_0</v>
-      </c>
-      <c r="D5" s="2" t="str">
-        <f>CONCATENATE(B5," - Attribute 0")</f>
-        <v>Program Type 1 - Attribute 0</v>
-      </c>
-    </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.45">
-      <c r="C6" s="2" t="str">
-        <f>CONCATENATE(A5,"_att_1")</f>
-        <v>progtype_1_att_1</v>
-      </c>
-      <c r="D6" s="2" t="str">
-        <f>CONCATENATE(B5," - Attribute 1")</f>
-        <v>Program Type 1 - Attribute 1</v>
-      </c>
-    </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.45">
-      <c r="C7" s="2" t="str">
-        <f>CONCATENATE(A5,"_att_2")</f>
-        <v>progtype_1_att_2</v>
-      </c>
-      <c r="D7" s="2" t="str">
-        <f>CONCATENATE(B5," - Attribute 2")</f>
-        <v>Program Type 1 - Attribute 2</v>
-      </c>
-    </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.45">
-      <c r="A8" s="2" t="s">
-        <v>18</v>
-      </c>
-      <c r="B8" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="C8" s="2" t="str">
-        <f>CONCATENATE(A8,"_att_0")</f>
-        <v>progtype_2_att_0</v>
-      </c>
-      <c r="D8" s="2" t="str">
-        <f>CONCATENATE(B8," - Attribute 0")</f>
-        <v>Program Type 2 - Attribute 0</v>
-      </c>
-    </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.45">
-      <c r="C9" s="2" t="str">
-        <f>CONCATENATE(A8,"_att_1")</f>
-        <v>progtype_2_att_1</v>
-      </c>
-      <c r="D9" s="2" t="str">
-        <f>CONCATENATE(B8," - Attribute 1")</f>
-        <v>Program Type 2 - Attribute 1</v>
-      </c>
-    </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.45">
-      <c r="C10" s="2" t="str">
-        <f>CONCATENATE(A8,"_att_2")</f>
-        <v>progtype_2_att_2</v>
-      </c>
-      <c r="D10" s="2" t="str">
-        <f>CONCATENATE(B8," - Attribute 2")</f>
-        <v>Program Type 2 - Attribute 2</v>
-      </c>
-    </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.45">
-      <c r="A11" s="2" t="s">
-        <v>20</v>
-      </c>
-      <c r="B11" s="2" t="s">
-        <v>21</v>
-      </c>
-      <c r="C11" s="2" t="str">
-        <f>CONCATENATE(A11,"_att_0")</f>
-        <v>progtype_3_att_0</v>
-      </c>
-      <c r="D11" s="2" t="str">
-        <f>CONCATENATE(B11," - Attribute 0")</f>
-        <v>Program Type 3 - Attribute 0</v>
-      </c>
-    </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.45">
-      <c r="C12" s="2" t="str">
-        <f>CONCATENATE(A11,"_att_1")</f>
-        <v>progtype_3_att_1</v>
-      </c>
-      <c r="D12" s="2" t="str">
-        <f>CONCATENATE(B11," - Attribute 1")</f>
-        <v>Program Type 3 - Attribute 1</v>
-      </c>
-    </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.45">
-      <c r="C13" s="2" t="str">
-        <f>CONCATENATE(A11,"_att_2")</f>
-        <v>progtype_3_att_2</v>
-      </c>
-      <c r="D13" s="2" t="str">
-        <f>CONCATENATE(B11," - Attribute 2")</f>
-        <v>Program Type 3 - Attribute 2</v>
-      </c>
-    </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.45">
-      <c r="A14" s="2" t="s">
-        <v>22</v>
-      </c>
-      <c r="B14" s="2" t="s">
-        <v>23</v>
-      </c>
-      <c r="C14" s="2" t="str">
-        <f>CONCATENATE(A14,"_att_0")</f>
-        <v>progtype_4_att_0</v>
-      </c>
-      <c r="D14" s="2" t="str">
-        <f>CONCATENATE(B14," - Attribute 0")</f>
-        <v>Program Type 4 - Attribute 0</v>
-      </c>
-    </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.45">
-      <c r="C15" s="2" t="str">
-        <f>CONCATENATE(A14,"_att_1")</f>
-        <v>progtype_4_att_1</v>
-      </c>
-      <c r="D15" s="2" t="str">
-        <f>CONCATENATE(B14," - Attribute 1")</f>
-        <v>Program Type 4 - Attribute 1</v>
-      </c>
-    </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.45">
-      <c r="C16" s="2" t="str">
-        <f>CONCATENATE(A14,"_att_2")</f>
-        <v>progtype_4_att_2</v>
-      </c>
-      <c r="D16" s="2" t="str">
-        <f>CONCATENATE(B14," - Attribute 2")</f>
-        <v>Program Type 4 - Attribute 2</v>
-      </c>
-    </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.45">
-      <c r="A17" s="2" t="s">
-        <v>24</v>
-      </c>
-      <c r="B17" s="2" t="s">
-        <v>25</v>
-      </c>
-      <c r="C17" s="2" t="str">
-        <f>CONCATENATE(A17,"_att_0")</f>
-        <v>progtype_5_att_0</v>
-      </c>
-      <c r="D17" s="2" t="str">
-        <f>CONCATENATE(B17," - Attribute 0")</f>
-        <v>Program Type 5 - Attribute 0</v>
-      </c>
-    </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.45">
-      <c r="C18" s="2" t="str">
-        <f>CONCATENATE(A17,"_att_1")</f>
-        <v>progtype_5_att_1</v>
-      </c>
-      <c r="D18" s="2" t="str">
-        <f>CONCATENATE(B17," - Attribute 1")</f>
-        <v>Program Type 5 - Attribute 1</v>
-      </c>
-    </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.45">
-      <c r="C19" s="2" t="str">
-        <f>CONCATENATE(A17,"_att_2")</f>
-        <v>progtype_5_att_2</v>
-      </c>
-      <c r="D19" s="2" t="str">
-        <f>CONCATENATE(B17," - Attribute 2")</f>
-        <v>Program Type 5 - Attribute 2</v>
-      </c>
-    </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.45">
-      <c r="A20" s="2" t="s">
-        <v>26</v>
-      </c>
-      <c r="B20" s="2" t="s">
-        <v>27</v>
-      </c>
-      <c r="C20" s="2" t="str">
-        <f>CONCATENATE(A20,"_att_0")</f>
-        <v>progtype_6_att_0</v>
-      </c>
-      <c r="D20" s="2" t="str">
-        <f>CONCATENATE(B20," - Attribute 0")</f>
-        <v>Program Type 6 - Attribute 0</v>
-      </c>
-    </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.45">
-      <c r="C21" s="2" t="str">
-        <f>CONCATENATE(A20,"_att_1")</f>
-        <v>progtype_6_att_1</v>
-      </c>
-      <c r="D21" s="2" t="str">
-        <f>CONCATENATE(B20," - Attribute 1")</f>
-        <v>Program Type 6 - Attribute 1</v>
-      </c>
-    </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.45">
-      <c r="C22" s="2" t="str">
-        <f>CONCATENATE(A20,"_att_2")</f>
-        <v>progtype_6_att_2</v>
-      </c>
-      <c r="D22" s="2" t="str">
-        <f>CONCATENATE(B20," - Attribute 2")</f>
-        <v>Program Type 6 - Attribute 2</v>
-      </c>
-    </row>
-  </sheetData>
+  <dataValidations count="1">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D2:D7" xr:uid="{38185FA4-540E-44B8-A8FE-03704A97DB42}">
+      <formula1>"n,y"</formula1>
+    </dataValidation>
+  </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <legacyDrawing r:id="rId1"/>
 </worksheet>

</xml_diff>

<commit_message>
Limit columns introduced for parameters
A 'Maximum Value' and 'Minimum Value' are now available in the parameters sheet of the framework file.
Inserted values are not currently used in the project.
</commit_message>
<xml_diff>
--- a/tests/frameworks/framework_sir.xlsx
+++ b/tests/frameworks/framework_sir.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Projects - Work\Optima\atomica\tests\frameworks\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D5F5411F-FE0D-47CA-BD25-7CEBFD11B4F1}" xr6:coauthVersionLast="32" xr6:coauthVersionMax="32" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ED106741-9EA2-4EF5-AF78-C2A83043C643}" xr6:coauthVersionLast="32" xr6:coauthVersionMax="32" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="240" yWindow="15" windowWidth="16095" windowHeight="9660" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -473,7 +473,33 @@
         </r>
       </text>
     </comment>
-    <comment ref="G1" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0300-000005000000}">
+    <comment ref="G1" authorId="0" shapeId="0" xr:uid="{8504EC81-F7D0-4EEA-A55E-83E0200D20F4}">
+      <text>
+        <r>
+          <rPr>
+            <sz val="8"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>This column defines a 'min' attribute for a 'par' item.</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="H1" authorId="0" shapeId="0" xr:uid="{959A03CA-9096-4C58-BFFA-B9A9C555B7D6}">
+      <text>
+        <r>
+          <rPr>
+            <sz val="8"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>This column defines a 'max' attribute for a 'par' item.</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="I1" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0300-000005000000}">
       <text>
         <r>
           <rPr>
@@ -491,7 +517,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="99" uniqueCount="59">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="101" uniqueCount="61">
   <si>
     <t>Code Name</t>
   </si>
@@ -668,6 +694,12 @@
   </si>
   <si>
     <t>Is Impact</t>
+  </si>
+  <si>
+    <t>Minimum Value</t>
+  </si>
+  <si>
+    <t>Maximum Value</t>
   </si>
 </sst>
 </file>
@@ -1497,10 +1529,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
-  <dimension ref="A1:G7"/>
+  <dimension ref="A1:I7"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E12" sqref="E12"/>
+    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="G1" sqref="A1:XFD1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -1511,10 +1543,12 @@
     <col min="4" max="4" width="8.1328125" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="13.86328125" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="11.73046875" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="96.33203125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="13.796875" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="14.06640625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="96.59765625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1534,10 +1568,16 @@
         <v>9</v>
       </c>
       <c r="G1" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="I1" s="1" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A2" s="3" t="s">
         <v>44</v>
       </c>
@@ -1554,9 +1594,11 @@
       <c r="F2" s="6">
         <v>8.0000000000000004E-4</v>
       </c>
-      <c r="G2" s="7"/>
-    </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="G2" s="2"/>
+      <c r="H2" s="2"/>
+      <c r="I2" s="7"/>
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A3" s="3" t="s">
         <v>46</v>
       </c>
@@ -1573,9 +1615,11 @@
       <c r="F3">
         <v>80</v>
       </c>
-      <c r="G3" s="7"/>
-    </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="G3" s="2"/>
+      <c r="H3" s="2"/>
+      <c r="I3" s="7"/>
+    </row>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A4" s="3" t="s">
         <v>21</v>
       </c>
@@ -1591,11 +1635,13 @@
       <c r="E4" s="2">
         <v>-1</v>
       </c>
-      <c r="G4" s="7" t="s">
+      <c r="G4" s="2"/>
+      <c r="H4" s="2"/>
+      <c r="I4" s="7" t="s">
         <v>57</v>
       </c>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="5" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A5" s="3" t="s">
         <v>23</v>
       </c>
@@ -1612,9 +1658,11 @@
       <c r="F5">
         <v>0.5</v>
       </c>
-      <c r="G5" s="7"/>
-    </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="G5" s="2"/>
+      <c r="H5" s="2"/>
+      <c r="I5" s="7"/>
+    </row>
+    <row r="6" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A6" s="3" t="s">
         <v>24</v>
       </c>
@@ -1631,9 +1679,11 @@
       <c r="F6" s="8">
         <v>1.6E-2</v>
       </c>
-      <c r="G6" s="7"/>
-    </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="G6" s="2"/>
+      <c r="H6" s="2"/>
+      <c r="I6" s="7"/>
+    </row>
+    <row r="7" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A7" s="3" t="s">
         <v>22</v>
       </c>
@@ -1650,7 +1700,9 @@
       <c r="F7" s="8">
         <v>8.0000000000000002E-3</v>
       </c>
-      <c r="G7" s="7"/>
+      <c r="G7" s="2"/>
+      <c r="H7" s="2"/>
+      <c r="I7" s="7"/>
     </row>
   </sheetData>
   <dataValidations count="1">

</xml_diff>

<commit_message>
Databook updated to work with framework
A corresponding databook has been constructed for the SIR framework.
However, review must continue as test results are not as expected.
</commit_message>
<xml_diff>
--- a/tests/frameworks/framework_sir.xlsx
+++ b/tests/frameworks/framework_sir.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Projects - Work\Optima\atomica\tests\frameworks\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ED106741-9EA2-4EF5-AF78-C2A83043C643}" xr6:coauthVersionLast="32" xr6:coauthVersionMax="32" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8E75C012-AB74-45E3-A2E0-E5A6FF5E789B}" xr6:coauthVersionLast="32" xr6:coauthVersionMax="32" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="15" windowWidth="16095" windowHeight="9660" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="240" yWindow="15" windowWidth="16095" windowHeight="9660" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Compartments" sheetId="1" r:id="rId1"/>
@@ -517,7 +517,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="101" uniqueCount="61">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="161" uniqueCount="97">
   <si>
     <t>Code Name</t>
   </si>
@@ -669,18 +669,12 @@
     <t>Force of infection</t>
   </si>
   <si>
-    <t>Average duration of infections (years)</t>
-  </si>
-  <si>
     <t>Duration</t>
   </si>
   <si>
     <t>Death rate for infected people</t>
   </si>
   <si>
-    <t>Death rate for susceptible people</t>
-  </si>
-  <si>
     <t>Setup Weight</t>
   </si>
   <si>
@@ -700,6 +694,120 @@
   </si>
   <si>
     <t>Maximum Value</t>
+  </si>
+  <si>
+    <t>cov_avoid</t>
+  </si>
+  <si>
+    <t>cov_reduc</t>
+  </si>
+  <si>
+    <t>cov_treat</t>
+  </si>
+  <si>
+    <t>Coverage by risk avoidance programs</t>
+  </si>
+  <si>
+    <t>Coverage by harm reduction programs</t>
+  </si>
+  <si>
+    <t>Coverage by treatment programs</t>
+  </si>
+  <si>
+    <t>suff_avoid</t>
+  </si>
+  <si>
+    <t>suff_reduc</t>
+  </si>
+  <si>
+    <t>suff_treat</t>
+  </si>
+  <si>
+    <t>Coverage sufficiency of risk avoidance programs</t>
+  </si>
+  <si>
+    <t>Coverage sufficiency of harm reduction programs</t>
+  </si>
+  <si>
+    <t>Coverage sufficiency of treatment programs</t>
+  </si>
+  <si>
+    <t>tpc_uncov</t>
+  </si>
+  <si>
+    <t>ctc_uncov</t>
+  </si>
+  <si>
+    <t>rec_uncov</t>
+  </si>
+  <si>
+    <t>ded_uncov</t>
+  </si>
+  <si>
+    <t>tpc_cov</t>
+  </si>
+  <si>
+    <t>ctc_cov</t>
+  </si>
+  <si>
+    <t>rec_cov</t>
+  </si>
+  <si>
+    <t>ded_cov</t>
+  </si>
+  <si>
+    <t>cov_avoid/sus</t>
+  </si>
+  <si>
+    <t>cov_reduc/sus</t>
+  </si>
+  <si>
+    <t>cov_treat/inf</t>
+  </si>
+  <si>
+    <t>Transmission probability per contact (worst case)</t>
+  </si>
+  <si>
+    <t>Transmission probability per contact (best case)</t>
+  </si>
+  <si>
+    <t>Number of contacts annually (worst case)</t>
+  </si>
+  <si>
+    <t>Number of contacts annually (best case)</t>
+  </si>
+  <si>
+    <t>Average duration of infections in years (best case)</t>
+  </si>
+  <si>
+    <t>Average duration of infections in years (worst case)</t>
+  </si>
+  <si>
+    <t>Death rate for infected people (worst case)</t>
+  </si>
+  <si>
+    <t>Death rate for infected people (best case)</t>
+  </si>
+  <si>
+    <t>Average duration of infections in years</t>
+  </si>
+  <si>
+    <t>ctc_cov*suff_avoid+ctc_uncov*(1-suff_avoid)</t>
+  </si>
+  <si>
+    <t>tpc_cov*suff_reduc+tpc_uncov*(1-suff_reduc)</t>
+  </si>
+  <si>
+    <t>rec_cov*suff_treat+rec_uncov*(1-suff_treat)</t>
+  </si>
+  <si>
+    <t>ded_cov*suff_treat+ded_uncov*(1-suff_treat)</t>
+  </si>
+  <si>
+    <t>Normal death rate</t>
+  </si>
+  <si>
+    <t>susdeath, infdeath</t>
   </si>
 </sst>
 </file>
@@ -772,9 +880,11 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1145,7 +1255,7 @@
         <v>8</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.45">
@@ -1253,13 +1363,13 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:E5"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B2" sqref="A1:E5"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E3" sqref="E3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
-    <col min="5" max="5" width="7.73046875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="14.86328125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.45">
@@ -1301,7 +1411,7 @@
         <v>23</v>
       </c>
       <c r="E3" t="s">
-        <v>24</v>
+        <v>96</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.45">
@@ -1353,7 +1463,7 @@
         <v>8</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="E1" s="1" t="s">
         <v>6</v>
@@ -1384,10 +1494,10 @@
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A3" s="4" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="B3" s="4" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="C3" s="2"/>
       <c r="D3" s="2">
@@ -1529,20 +1639,20 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
-  <dimension ref="A1:I7"/>
+  <dimension ref="A1:I21"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="G1" sqref="A1:XFD1048576"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B9" sqref="B9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
     <col min="1" max="1" width="13.265625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="30.6640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="41.59765625" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="9.265625" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="8.1328125" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="13.86328125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="11.73046875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="11.73046875" style="8" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="13.796875" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="14.06640625" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="96.59765625" bestFit="1" customWidth="1"/>
@@ -1559,19 +1669,19 @@
         <v>10</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="E1" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="F1" s="7" t="s">
         <v>9</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="H1" s="1" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="I1" s="1" t="s">
         <v>11</v>
@@ -1579,138 +1689,428 @@
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A2" s="3" t="s">
-        <v>44</v>
+        <v>59</v>
       </c>
       <c r="B2" s="5" t="s">
-        <v>45</v>
+        <v>62</v>
       </c>
       <c r="C2" t="s">
-        <v>43</v>
+        <v>48</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>5</v>
+        <v>20</v>
       </c>
       <c r="E2" s="2"/>
-      <c r="F2" s="6">
-        <v>8.0000000000000004E-4</v>
-      </c>
       <c r="G2" s="2"/>
       <c r="H2" s="2"/>
-      <c r="I2" s="7"/>
+      <c r="I2" s="6"/>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A3" s="3" t="s">
-        <v>46</v>
+        <v>60</v>
       </c>
       <c r="B3" s="5" t="s">
-        <v>47</v>
+        <v>63</v>
       </c>
       <c r="C3" t="s">
         <v>48</v>
       </c>
       <c r="D3" s="2" t="s">
-        <v>5</v>
+        <v>20</v>
       </c>
       <c r="E3" s="2"/>
-      <c r="F3">
-        <v>80</v>
-      </c>
       <c r="G3" s="2"/>
       <c r="H3" s="2"/>
-      <c r="I3" s="7"/>
+      <c r="I3" s="6"/>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A4" s="3" t="s">
-        <v>21</v>
+        <v>61</v>
       </c>
       <c r="B4" s="5" t="s">
-        <v>49</v>
+        <v>64</v>
       </c>
       <c r="C4" t="s">
-        <v>43</v>
+        <v>48</v>
       </c>
       <c r="D4" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="E4" s="2">
-        <v>-1</v>
-      </c>
+        <v>20</v>
+      </c>
+      <c r="E4" s="2"/>
       <c r="G4" s="2"/>
       <c r="H4" s="2"/>
-      <c r="I4" s="7" t="s">
-        <v>57</v>
-      </c>
+      <c r="I4" s="6"/>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A5" s="3" t="s">
-        <v>23</v>
+        <v>65</v>
       </c>
       <c r="B5" s="5" t="s">
-        <v>50</v>
-      </c>
-      <c r="C5" t="s">
-        <v>51</v>
+        <v>68</v>
       </c>
       <c r="D5" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="E5" s="2"/>
-      <c r="F5">
-        <v>0.5</v>
+      <c r="E5" s="2">
+        <v>-1</v>
       </c>
       <c r="G5" s="2"/>
-      <c r="H5" s="2"/>
-      <c r="I5" s="7"/>
+      <c r="H5" s="2">
+        <v>1</v>
+      </c>
+      <c r="I5" s="6" t="s">
+        <v>79</v>
+      </c>
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A6" s="3" t="s">
-        <v>24</v>
+        <v>66</v>
       </c>
       <c r="B6" s="5" t="s">
-        <v>52</v>
-      </c>
-      <c r="C6" t="s">
-        <v>43</v>
+        <v>69</v>
       </c>
       <c r="D6" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="E6" s="2"/>
-      <c r="F6" s="8">
-        <v>1.6E-2</v>
+      <c r="E6" s="2">
+        <v>-1</v>
       </c>
       <c r="G6" s="2"/>
-      <c r="H6" s="2"/>
-      <c r="I6" s="7"/>
+      <c r="H6" s="2">
+        <v>1</v>
+      </c>
+      <c r="I6" s="6" t="s">
+        <v>80</v>
+      </c>
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A7" s="3" t="s">
+        <v>67</v>
+      </c>
+      <c r="B7" s="5" t="s">
+        <v>70</v>
+      </c>
+      <c r="D7" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="E7" s="2">
+        <v>-1</v>
+      </c>
+      <c r="G7" s="2"/>
+      <c r="H7" s="2">
+        <v>1</v>
+      </c>
+      <c r="I7" s="6" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9" x14ac:dyDescent="0.45">
+      <c r="A8" s="3" t="s">
         <v>22</v>
       </c>
-      <c r="B7" s="5" t="s">
-        <v>53</v>
-      </c>
-      <c r="C7" t="s">
+      <c r="B8" s="5" t="s">
+        <v>95</v>
+      </c>
+      <c r="C8" t="s">
         <v>43</v>
       </c>
-      <c r="D7" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="E7" s="2"/>
-      <c r="F7" s="8">
+      <c r="D8" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="E8" s="2"/>
+      <c r="F8" s="8">
         <v>8.0000000000000002E-3</v>
       </c>
-      <c r="G7" s="2"/>
-      <c r="H7" s="2"/>
-      <c r="I7" s="7"/>
+      <c r="G8" s="2"/>
+      <c r="H8" s="2"/>
+      <c r="I8" s="6"/>
+    </row>
+    <row r="9" spans="1:9" x14ac:dyDescent="0.45">
+      <c r="A9" s="3" t="s">
+        <v>71</v>
+      </c>
+      <c r="B9" s="5" t="s">
+        <v>82</v>
+      </c>
+      <c r="C9" t="s">
+        <v>43</v>
+      </c>
+      <c r="D9" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="E9" s="2"/>
+      <c r="F9" s="8">
+        <v>8.0000000000000004E-4</v>
+      </c>
+      <c r="G9" s="2"/>
+      <c r="H9" s="2"/>
+      <c r="I9" s="6"/>
+    </row>
+    <row r="10" spans="1:9" x14ac:dyDescent="0.45">
+      <c r="A10" s="3" t="s">
+        <v>75</v>
+      </c>
+      <c r="B10" s="5" t="s">
+        <v>83</v>
+      </c>
+      <c r="C10" t="s">
+        <v>43</v>
+      </c>
+      <c r="D10" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="E10" s="2"/>
+      <c r="F10" s="8">
+        <v>1E-4</v>
+      </c>
+      <c r="G10" s="2"/>
+      <c r="H10" s="2"/>
+      <c r="I10" s="6"/>
+    </row>
+    <row r="11" spans="1:9" x14ac:dyDescent="0.45">
+      <c r="A11" s="3" t="s">
+        <v>72</v>
+      </c>
+      <c r="B11" s="5" t="s">
+        <v>84</v>
+      </c>
+      <c r="C11" t="s">
+        <v>48</v>
+      </c>
+      <c r="D11" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="E11" s="2"/>
+      <c r="F11" s="8">
+        <v>80</v>
+      </c>
+      <c r="G11" s="2"/>
+      <c r="H11" s="2"/>
+      <c r="I11" s="6"/>
+    </row>
+    <row r="12" spans="1:9" x14ac:dyDescent="0.45">
+      <c r="A12" s="3" t="s">
+        <v>76</v>
+      </c>
+      <c r="B12" s="5" t="s">
+        <v>85</v>
+      </c>
+      <c r="C12" t="s">
+        <v>48</v>
+      </c>
+      <c r="D12" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="E12" s="2"/>
+      <c r="F12" s="8">
+        <v>20</v>
+      </c>
+      <c r="G12" s="2"/>
+      <c r="H12" s="2"/>
+      <c r="I12" s="6"/>
+    </row>
+    <row r="13" spans="1:9" x14ac:dyDescent="0.45">
+      <c r="A13" s="3" t="s">
+        <v>73</v>
+      </c>
+      <c r="B13" s="5" t="s">
+        <v>87</v>
+      </c>
+      <c r="C13" t="s">
+        <v>50</v>
+      </c>
+      <c r="D13" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="E13" s="2"/>
+      <c r="F13" s="8">
+        <v>0.5</v>
+      </c>
+      <c r="G13" s="2"/>
+      <c r="H13" s="2"/>
+      <c r="I13" s="6"/>
+    </row>
+    <row r="14" spans="1:9" x14ac:dyDescent="0.45">
+      <c r="A14" s="3" t="s">
+        <v>77</v>
+      </c>
+      <c r="B14" s="5" t="s">
+        <v>86</v>
+      </c>
+      <c r="C14" t="s">
+        <v>50</v>
+      </c>
+      <c r="D14" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="E14" s="2"/>
+      <c r="F14" s="8">
+        <v>0.25</v>
+      </c>
+      <c r="G14" s="2"/>
+      <c r="H14" s="2"/>
+      <c r="I14" s="6"/>
+    </row>
+    <row r="15" spans="1:9" x14ac:dyDescent="0.45">
+      <c r="A15" s="3" t="s">
+        <v>74</v>
+      </c>
+      <c r="B15" s="5" t="s">
+        <v>88</v>
+      </c>
+      <c r="C15" t="s">
+        <v>43</v>
+      </c>
+      <c r="D15" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="E15" s="2"/>
+      <c r="F15" s="8">
+        <v>1.6E-2</v>
+      </c>
+      <c r="G15" s="2"/>
+      <c r="H15" s="2"/>
+      <c r="I15" s="6"/>
+    </row>
+    <row r="16" spans="1:9" x14ac:dyDescent="0.45">
+      <c r="A16" s="3" t="s">
+        <v>78</v>
+      </c>
+      <c r="B16" s="5" t="s">
+        <v>89</v>
+      </c>
+      <c r="C16" t="s">
+        <v>43</v>
+      </c>
+      <c r="D16" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="E16" s="2"/>
+      <c r="F16" s="8">
+        <v>1.2E-2</v>
+      </c>
+      <c r="G16" s="2"/>
+      <c r="H16" s="2"/>
+      <c r="I16" s="6"/>
+    </row>
+    <row r="17" spans="1:9" x14ac:dyDescent="0.45">
+      <c r="A17" s="3" t="s">
+        <v>44</v>
+      </c>
+      <c r="B17" s="5" t="s">
+        <v>45</v>
+      </c>
+      <c r="C17" t="s">
+        <v>43</v>
+      </c>
+      <c r="D17" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="E17" s="2">
+        <v>-1</v>
+      </c>
+      <c r="G17" s="2"/>
+      <c r="H17" s="2"/>
+      <c r="I17" s="6" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="18" spans="1:9" x14ac:dyDescent="0.45">
+      <c r="A18" s="3" t="s">
+        <v>46</v>
+      </c>
+      <c r="B18" s="5" t="s">
+        <v>47</v>
+      </c>
+      <c r="C18" t="s">
+        <v>48</v>
+      </c>
+      <c r="D18" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="E18" s="2">
+        <v>-1</v>
+      </c>
+      <c r="G18" s="2"/>
+      <c r="H18" s="2"/>
+      <c r="I18" s="6" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="19" spans="1:9" x14ac:dyDescent="0.45">
+      <c r="A19" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="B19" s="5" t="s">
+        <v>90</v>
+      </c>
+      <c r="C19" t="s">
+        <v>50</v>
+      </c>
+      <c r="D19" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="E19" s="2">
+        <v>-1</v>
+      </c>
+      <c r="G19" s="2"/>
+      <c r="H19" s="2"/>
+      <c r="I19" s="6" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="20" spans="1:9" x14ac:dyDescent="0.45">
+      <c r="A20" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="B20" s="5" t="s">
+        <v>51</v>
+      </c>
+      <c r="C20" t="s">
+        <v>43</v>
+      </c>
+      <c r="D20" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="E20" s="2">
+        <v>-1</v>
+      </c>
+      <c r="G20" s="2"/>
+      <c r="H20" s="2"/>
+      <c r="I20" s="6" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="21" spans="1:9" x14ac:dyDescent="0.45">
+      <c r="A21" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="B21" s="5" t="s">
+        <v>49</v>
+      </c>
+      <c r="C21" t="s">
+        <v>43</v>
+      </c>
+      <c r="D21" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="E21" s="2">
+        <v>-1</v>
+      </c>
+      <c r="G21" s="2"/>
+      <c r="H21" s="2"/>
+      <c r="I21" s="6" t="s">
+        <v>55</v>
+      </c>
     </row>
   </sheetData>
   <dataValidations count="1">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D2:D7" xr:uid="{38185FA4-540E-44B8-A8FE-03704A97DB42}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D2:D21" xr:uid="{38185FA4-540E-44B8-A8FE-03704A97DB42}">
       <formula1>"n,y"</formula1>
     </dataValidation>
   </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <legacyDrawing r:id="rId1"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+  <legacyDrawing r:id="rId2"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Preparations for data plotting
</commit_message>
<xml_diff>
--- a/tests/frameworks/framework_sir.xlsx
+++ b/tests/frameworks/framework_sir.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="20228"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="20325"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\projects\atomica\atomica\tests\frameworks\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CCF627C6-6EC0-488E-969D-42B98A37CF3D}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C3D4E142-9F6A-4AEE-AE4D-58A205E36913}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="15" windowWidth="16095" windowHeight="9660" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="240" yWindow="15" windowWidth="16095" windowHeight="9660" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Databook Pages" sheetId="5" r:id="rId1"/>
@@ -20,7 +20,7 @@
     <sheet name="Parameters" sheetId="4" r:id="rId5"/>
     <sheet name="Cascades" sheetId="6" r:id="rId6"/>
   </sheets>
-  <calcPr calcId="179017"/>
+  <calcPr calcId="179021"/>
 </workbook>
 </file>
 
@@ -726,10 +726,10 @@
     <t>Constituents</t>
   </si>
   <si>
-    <t>sus+inf+rec</t>
-  </si>
-  <si>
-    <t>inf+rec</t>
+    <t>sus,inf,rec</t>
+  </si>
+  <si>
+    <t>inf,rec</t>
   </si>
 </sst>
 </file>
@@ -1221,7 +1221,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:H5"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="S17" sqref="S17"/>
     </sheetView>
   </sheetViews>
@@ -1438,7 +1438,7 @@
   <dimension ref="A1:H9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="I1" sqref="I1:I1048576"/>
+      <selection activeCell="F11" sqref="F11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1447,7 +1447,7 @@
     <col min="2" max="2" width="27.7109375" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="27.7109375" customWidth="1"/>
     <col min="4" max="5" width="20.7109375" customWidth="1"/>
-    <col min="6" max="6" width="11.140625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="12.28515625" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="11.5703125" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="11.7109375" bestFit="1" customWidth="1"/>
   </cols>
@@ -1785,13 +1785,14 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E94509DB-A1F5-4668-BF8F-11287B88AAAB}">
   <dimension ref="A1:B4"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E14" sqref="E14"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B2" sqref="B2:B4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="22.85546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="12.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
@@ -1806,7 +1807,7 @@
       <c r="A2" s="4" t="s">
         <v>26</v>
       </c>
-      <c r="B2" s="3" t="s">
+      <c r="B2" t="s">
         <v>68</v>
       </c>
     </row>
@@ -1814,7 +1815,7 @@
       <c r="A3" s="3" t="s">
         <v>29</v>
       </c>
-      <c r="B3" s="3" t="s">
+      <c r="B3" t="s">
         <v>69</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Auto-calibration works again for SIR and TB
</commit_message>
<xml_diff>
--- a/tests/frameworks/framework_sir.xlsx
+++ b/tests/frameworks/framework_sir.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\projects\atomica\atomica\tests\frameworks\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4A1BEF3F-E0F0-4F4B-8686-5A808659E25D}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5C258852-032C-469C-ACC4-30DD3006EBB7}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="15" windowWidth="16095" windowHeight="9660" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="240" yWindow="15" windowWidth="16095" windowHeight="9660" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Databook Pages" sheetId="5" r:id="rId1"/>
@@ -476,7 +476,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="D1" authorId="0" shapeId="0" xr:uid="{65E32CD1-EF29-4034-8FD9-2B2CA808AD0D}">
+    <comment ref="F1" authorId="0" shapeId="0" xr:uid="{65E32CD1-EF29-4034-8FD9-2B2CA808AD0D}">
       <text>
         <r>
           <rPr>
@@ -489,7 +489,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="E1" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0300-000004000000}">
+    <comment ref="G1" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0300-000004000000}">
       <text>
         <r>
           <rPr>
@@ -502,7 +502,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="F1" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0300-000005000000}">
+    <comment ref="H1" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0300-000005000000}">
       <text>
         <r>
           <rPr>
@@ -520,7 +520,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="111" uniqueCount="69">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="123" uniqueCount="70">
   <si>
     <t>Code Name</t>
   </si>
@@ -727,6 +727,9 @@
   </si>
   <si>
     <t>inf,rec</t>
+  </si>
+  <si>
+    <t>Is Impact</t>
   </si>
 </sst>
 </file>
@@ -1144,7 +1147,7 @@
   <dimension ref="A1:B11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D20" sqref="D20"/>
+      <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1639,23 +1642,25 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
-  <dimension ref="A1:F7"/>
+  <dimension ref="A1:H7"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D20" sqref="D20"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E10" sqref="E10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="13.28515625" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="30.7109375" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="9.28515625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="13.85546875" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="11.7109375" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="96.28515625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="10.7109375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="14.28515625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="14.28515625" customWidth="1"/>
+    <col min="6" max="6" width="20.5703125" customWidth="1"/>
+    <col min="7" max="7" width="11.7109375" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="96.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1666,16 +1671,22 @@
         <v>10</v>
       </c>
       <c r="D1" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="F1" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="G1" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="H1" s="1" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A2" s="3" t="s">
         <v>44</v>
       </c>
@@ -1685,13 +1696,19 @@
       <c r="C2" t="s">
         <v>43</v>
       </c>
-      <c r="D2" s="2"/>
-      <c r="E2" s="6">
+      <c r="D2" s="2" t="s">
+        <v>63</v>
+      </c>
+      <c r="E2" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="F2" s="2"/>
+      <c r="G2" s="6">
         <v>8.0000000000000004E-4</v>
       </c>
-      <c r="F2" s="7"/>
-    </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="H2" s="7"/>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A3" s="3" t="s">
         <v>46</v>
       </c>
@@ -1701,13 +1718,19 @@
       <c r="C3" t="s">
         <v>48</v>
       </c>
-      <c r="D3" s="2"/>
-      <c r="E3">
+      <c r="D3" s="2" t="s">
+        <v>63</v>
+      </c>
+      <c r="E3" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="F3" s="2"/>
+      <c r="G3">
         <v>80</v>
       </c>
-      <c r="F3" s="7"/>
-    </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="H3" s="7"/>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A4" s="3" t="s">
         <v>21</v>
       </c>
@@ -1717,14 +1740,14 @@
       <c r="C4" t="s">
         <v>43</v>
       </c>
-      <c r="D4" s="2">
-        <v>-1</v>
-      </c>
-      <c r="F4" s="7" t="s">
+      <c r="D4" s="2"/>
+      <c r="E4" s="2"/>
+      <c r="F4" s="2"/>
+      <c r="H4" s="7" t="s">
         <v>57</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A5" s="3" t="s">
         <v>23</v>
       </c>
@@ -1734,13 +1757,19 @@
       <c r="C5" t="s">
         <v>51</v>
       </c>
-      <c r="D5" s="2"/>
-      <c r="E5">
+      <c r="D5" s="2" t="s">
+        <v>63</v>
+      </c>
+      <c r="E5" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="F5" s="2"/>
+      <c r="G5">
         <v>0.5</v>
       </c>
-      <c r="F5" s="7"/>
-    </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="H5" s="7"/>
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A6" s="3" t="s">
         <v>24</v>
       </c>
@@ -1750,13 +1779,19 @@
       <c r="C6" t="s">
         <v>43</v>
       </c>
-      <c r="D6" s="2"/>
-      <c r="E6" s="8">
+      <c r="D6" s="2" t="s">
+        <v>63</v>
+      </c>
+      <c r="E6" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="F6" s="2"/>
+      <c r="G6" s="8">
         <v>1.6E-2</v>
       </c>
-      <c r="F6" s="7"/>
-    </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="H6" s="7"/>
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A7" s="3" t="s">
         <v>22</v>
       </c>
@@ -1766,11 +1801,17 @@
       <c r="C7" t="s">
         <v>43</v>
       </c>
-      <c r="D7" s="2"/>
-      <c r="E7" s="8">
+      <c r="D7" s="2" t="s">
+        <v>63</v>
+      </c>
+      <c r="E7" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="F7" s="2"/>
+      <c r="G7" s="8">
         <v>8.0000000000000002E-3</v>
       </c>
-      <c r="F7" s="7"/>
+      <c r="H7" s="7"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -1782,7 +1823,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E94509DB-A1F5-4668-BF8F-11287B88AAAB}">
   <dimension ref="A1:B4"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
Added additional parameter validation
</commit_message>
<xml_diff>
--- a/tests/frameworks/framework_sir.xlsx
+++ b/tests/frameworks/framework_sir.xlsx
@@ -1,16 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="20325"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\projects\atomica\atomica\tests\frameworks\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\romesh.abey\Desktop\projects\atomica\atomica\tests\frameworks\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A11A6525-A2C1-4FC3-99E4-40914F58C2A0}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="465" windowWidth="16095" windowHeight="9660" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="240" yWindow="468" windowWidth="16098" windowHeight="9660" activeTab="5"/>
   </bookViews>
   <sheets>
     <sheet name="About" sheetId="7" r:id="rId1"/>
@@ -21,17 +20,17 @@
     <sheet name="Parameters" sheetId="4" r:id="rId6"/>
     <sheet name="Cascades" sheetId="6" r:id="rId7"/>
   </sheets>
-  <calcPr calcId="179021"/>
+  <calcPr calcId="162913"/>
 </workbook>
 </file>
 
 <file path=xl/comments1.xml><?xml version="1.0" encoding="utf-8"?>
-<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <authors>
     <author/>
   </authors>
   <commentList>
-    <comment ref="A1" authorId="0" shapeId="0" xr:uid="{A933BB2F-BD44-4AA3-9747-9EE271A8A43E}">
+    <comment ref="A1" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -52,7 +51,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="B1" authorId="0" shapeId="0" xr:uid="{2C9FAE90-07ED-44EF-9D3B-D0E0456BD991}">
+    <comment ref="B1" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -75,12 +74,12 @@
 </file>
 
 <file path=xl/comments2.xml><?xml version="1.0" encoding="utf-8"?>
-<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <authors>
     <author/>
   </authors>
   <commentList>
-    <comment ref="A1" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000001000000}">
+    <comment ref="A1" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -105,7 +104,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="B1" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000002000000}">
+    <comment ref="B1" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -131,7 +130,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="C1" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000003000000}">
+    <comment ref="C1" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -157,7 +156,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="D1" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000004000000}">
+    <comment ref="D1" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -182,7 +181,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="E1" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000005000000}">
+    <comment ref="E1" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -210,7 +209,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="G1" authorId="0" shapeId="0" xr:uid="{366F887C-C07F-4154-8785-9BDF4F8B6839}">
+    <comment ref="G1" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -225,7 +224,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="H1" authorId="0" shapeId="0" xr:uid="{3881AE7E-FAB1-4967-BFF9-35EC5F9DF654}">
+    <comment ref="H1" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -258,12 +257,12 @@
 </file>
 
 <file path=xl/comments3.xml><?xml version="1.0" encoding="utf-8"?>
-<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <authors>
     <author/>
   </authors>
   <commentList>
-    <comment ref="A1" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0200-000001000000}">
+    <comment ref="A1" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -288,7 +287,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="B1" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0200-000002000000}">
+    <comment ref="B1" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -314,7 +313,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="D1" authorId="0" shapeId="0" xr:uid="{CC0CB859-3F5D-43C9-94B0-27F5CB43D565}">
+    <comment ref="D1" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -329,7 +328,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="E1" authorId="0" shapeId="0" xr:uid="{A1CB8378-C4D4-4895-97A1-EAB67B145FFE}">
+    <comment ref="E1" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -356,7 +355,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="F1" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0200-000003000000}">
+    <comment ref="F1" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -383,7 +382,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="G1" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0200-000004000000}">
+    <comment ref="G1" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -396,7 +395,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="H1" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0200-000006000000}">
+    <comment ref="H1" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -414,12 +413,12 @@
 </file>
 
 <file path=xl/comments4.xml><?xml version="1.0" encoding="utf-8"?>
-<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <authors>
     <author/>
   </authors>
   <commentList>
-    <comment ref="A1" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0300-000001000000}">
+    <comment ref="A1" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -441,7 +440,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="B1" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0300-000002000000}">
+    <comment ref="B1" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -464,7 +463,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="C1" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0300-000003000000}">
+    <comment ref="C1" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -477,7 +476,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="F1" authorId="0" shapeId="0" xr:uid="{65E32CD1-EF29-4034-8FD9-2B2CA808AD0D}">
+    <comment ref="F1" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -490,7 +489,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="G1" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0300-000004000000}">
+    <comment ref="G1" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -503,7 +502,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="H1" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0300-000005000000}">
+    <comment ref="H1" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -748,7 +747,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -915,23 +914,6 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri" panose="020F0502020204030204"/>
@@ -967,23 +949,6 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -1159,16 +1124,16 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A224E424-D7C4-446D-A46F-73A4430DA45C}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="8.83984375" defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A1" s="9" t="s">
         <v>69</v>
       </c>
@@ -1176,7 +1141,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A2" s="10" t="s">
         <v>71</v>
       </c>
@@ -1190,19 +1155,19 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{158C4163-0781-4E11-A6B9-0912B33A6E99}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
   <cols>
-    <col min="1" max="2" width="25.7109375" customWidth="1"/>
+    <col min="1" max="2" width="25.68359375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A1" s="1" t="s">
         <v>62</v>
       </c>
@@ -1210,7 +1175,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A2" s="2" t="s">
         <v>59</v>
       </c>
@@ -1218,7 +1183,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A3" s="2" t="s">
         <v>63</v>
       </c>
@@ -1226,35 +1191,35 @@
         <v>65</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A4" s="2"/>
       <c r="B4" s="2"/>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A5" s="2"/>
       <c r="B5" s="2"/>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A6" s="2"/>
       <c r="B6" s="2"/>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A7" s="2"/>
       <c r="B7" s="2"/>
     </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A8" s="2"/>
       <c r="B8" s="2"/>
     </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A9" s="2"/>
       <c r="B9" s="2"/>
     </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A10" s="2"/>
       <c r="B10" s="2"/>
     </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A11" s="2"/>
       <c r="B11" s="2"/>
     </row>
@@ -1265,20 +1230,20 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="M8" sqref="M8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="8.83984375" defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
   <cols>
-    <col min="1" max="1" width="10.140625" bestFit="1" customWidth="1"/>
-    <col min="2" max="8" width="15.7109375" customWidth="1"/>
+    <col min="1" max="1" width="10.15625" bestFit="1" customWidth="1"/>
+    <col min="2" max="8" width="15.68359375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.55000000000000004">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1304,7 +1269,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.55000000000000004">
       <c r="A2" s="3" t="s">
         <v>12</v>
       </c>
@@ -1326,7 +1291,7 @@
       <c r="G2" s="2"/>
       <c r="H2" s="2"/>
     </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:8" x14ac:dyDescent="0.55000000000000004">
       <c r="A3" s="3" t="s">
         <v>14</v>
       </c>
@@ -1346,7 +1311,7 @@
       <c r="G3" s="2"/>
       <c r="H3" s="2"/>
     </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:8" x14ac:dyDescent="0.55000000000000004">
       <c r="A4" s="3" t="s">
         <v>16</v>
       </c>
@@ -1366,7 +1331,7 @@
       <c r="G4" s="2"/>
       <c r="H4" s="2"/>
     </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:8" x14ac:dyDescent="0.55000000000000004">
       <c r="A5" s="3" t="s">
         <v>18</v>
       </c>
@@ -1388,7 +1353,7 @@
     </row>
   </sheetData>
   <dataValidations count="1">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C2:E5" xr:uid="{EB410747-7D07-4683-B8BD-9F706D62D425}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C2:E5">
       <formula1>"n,y"</formula1>
     </dataValidation>
   </dataValidations>
@@ -1398,19 +1363,19 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="I8" sqref="I8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="8.83984375" defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
   <cols>
-    <col min="5" max="5" width="14.85546875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="14.83984375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="B1" s="1" t="str">
         <f>Compartments!A2</f>
         <v>sus</v>
@@ -1428,7 +1393,7 @@
         <v>dead</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A2" s="1" t="str">
         <f>Compartments!A2</f>
         <v>sus</v>
@@ -1440,7 +1405,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A3" s="1" t="str">
         <f>Compartments!A3</f>
         <v>inf</v>
@@ -1452,7 +1417,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A4" s="1" t="str">
         <f>Compartments!A4</f>
         <v>rec</v>
@@ -1461,7 +1426,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A5" s="1" t="str">
         <f>Compartments!A5</f>
         <v>dead</v>
@@ -1473,25 +1438,25 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="E19" sqref="E19"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="8.83984375" defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
   <cols>
-    <col min="1" max="1" width="12.42578125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="27.7109375" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="27.7109375" customWidth="1"/>
-    <col min="4" max="5" width="20.7109375" customWidth="1"/>
-    <col min="6" max="6" width="12.28515625" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="11.42578125" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="11.7109375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="12.41796875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="27.68359375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="27.68359375" customWidth="1"/>
+    <col min="4" max="5" width="20.68359375" customWidth="1"/>
+    <col min="6" max="6" width="12.26171875" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="11.41796875" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="11.68359375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.55000000000000004">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1517,7 +1482,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.55000000000000004">
       <c r="A2" s="4" t="s">
         <v>25</v>
       </c>
@@ -1535,7 +1500,7 @@
       <c r="G2" s="4"/>
       <c r="H2" s="2"/>
     </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:8" x14ac:dyDescent="0.55000000000000004">
       <c r="A3" s="4" t="s">
         <v>55</v>
       </c>
@@ -1555,7 +1520,7 @@
       </c>
       <c r="H3" s="2"/>
     </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:8" x14ac:dyDescent="0.55000000000000004">
       <c r="A4" s="3" t="s">
         <v>28</v>
       </c>
@@ -1571,7 +1536,7 @@
       <c r="G4" s="3"/>
       <c r="H4" s="2"/>
     </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:8" x14ac:dyDescent="0.55000000000000004">
       <c r="A5" s="3" t="s">
         <v>31</v>
       </c>
@@ -1587,7 +1552,7 @@
       <c r="G5" s="3"/>
       <c r="H5" s="2"/>
     </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:8" x14ac:dyDescent="0.55000000000000004">
       <c r="A6" s="3" t="s">
         <v>34</v>
       </c>
@@ -1603,7 +1568,7 @@
       <c r="G6" s="3"/>
       <c r="H6" s="2"/>
     </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:8" x14ac:dyDescent="0.55000000000000004">
       <c r="A7" s="3" t="s">
         <v>36</v>
       </c>
@@ -1621,7 +1586,7 @@
       </c>
       <c r="H7" s="2"/>
     </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:8" x14ac:dyDescent="0.55000000000000004">
       <c r="A8" s="3" t="s">
         <v>38</v>
       </c>
@@ -1639,7 +1604,7 @@
       </c>
       <c r="H8" s="2"/>
     </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:8" x14ac:dyDescent="0.55000000000000004">
       <c r="A9" s="3" t="s">
         <v>40</v>
       </c>
@@ -1664,26 +1629,26 @@
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E1" sqref="E1"/>
+      <selection activeCell="A4" sqref="A4:XFD4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="8.83984375" defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
   <cols>
-    <col min="1" max="1" width="13.28515625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="30.7109375" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="10.7109375" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="14.28515625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="14.28515625" customWidth="1"/>
-    <col min="6" max="6" width="20.42578125" customWidth="1"/>
-    <col min="7" max="7" width="11.7109375" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="96.28515625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="13.26171875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="30.68359375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="10.68359375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="14.26171875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="14.26171875" customWidth="1"/>
+    <col min="6" max="6" width="20.41796875" customWidth="1"/>
+    <col min="7" max="7" width="11.68359375" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="96.26171875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.55000000000000004">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1709,7 +1674,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.55000000000000004">
       <c r="A2" s="3" t="s">
         <v>44</v>
       </c>
@@ -1731,7 +1696,7 @@
       </c>
       <c r="H2" s="7"/>
     </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:8" x14ac:dyDescent="0.55000000000000004">
       <c r="A3" s="3" t="s">
         <v>46</v>
       </c>
@@ -1753,32 +1718,37 @@
       </c>
       <c r="H3" s="7"/>
     </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:8" x14ac:dyDescent="0.55000000000000004">
       <c r="A4" s="3" t="s">
-        <v>21</v>
+        <v>23</v>
       </c>
       <c r="B4" s="5" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="C4" t="s">
+        <v>51</v>
+      </c>
+      <c r="D4" s="2" t="s">
+        <v>63</v>
+      </c>
+      <c r="E4" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="F4" s="2"/>
+      <c r="G4">
+        <v>0.5</v>
+      </c>
+      <c r="H4" s="7"/>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.55000000000000004">
+      <c r="A5" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="B5" s="5" t="s">
+        <v>52</v>
+      </c>
+      <c r="C5" t="s">
         <v>43</v>
-      </c>
-      <c r="D4" s="2"/>
-      <c r="E4" s="2"/>
-      <c r="F4" s="2"/>
-      <c r="H4" s="7" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A5" s="3" t="s">
-        <v>23</v>
-      </c>
-      <c r="B5" s="5" t="s">
-        <v>50</v>
-      </c>
-      <c r="C5" t="s">
-        <v>51</v>
       </c>
       <c r="D5" s="2" t="s">
         <v>63</v>
@@ -1787,17 +1757,17 @@
         <v>20</v>
       </c>
       <c r="F5" s="2"/>
-      <c r="G5">
-        <v>0.5</v>
+      <c r="G5" s="8">
+        <v>1.6E-2</v>
       </c>
       <c r="H5" s="7"/>
     </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:8" x14ac:dyDescent="0.55000000000000004">
       <c r="A6" s="3" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="B6" s="5" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="C6" t="s">
         <v>43</v>
@@ -1810,31 +1780,26 @@
       </c>
       <c r="F6" s="2"/>
       <c r="G6" s="8">
-        <v>1.6E-2</v>
+        <v>8.0000000000000002E-3</v>
       </c>
       <c r="H6" s="7"/>
     </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:8" x14ac:dyDescent="0.55000000000000004">
       <c r="A7" s="3" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B7" s="5" t="s">
-        <v>53</v>
+        <v>49</v>
       </c>
       <c r="C7" t="s">
         <v>43</v>
       </c>
-      <c r="D7" s="2" t="s">
-        <v>63</v>
-      </c>
-      <c r="E7" s="2" t="s">
-        <v>20</v>
-      </c>
+      <c r="D7" s="2"/>
+      <c r="E7" s="2"/>
       <c r="F7" s="2"/>
-      <c r="G7" s="8">
-        <v>8.0000000000000002E-3</v>
-      </c>
-      <c r="H7" s="7"/>
+      <c r="H7" s="7" t="s">
+        <v>57</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -1843,20 +1808,20 @@
 </file>
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E94509DB-A1F5-4668-BF8F-11287B88AAAB}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="8.83984375" defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
   <cols>
-    <col min="1" max="1" width="22.85546875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="12.28515625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="22.83984375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="12.26171875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A1" s="9" t="s">
         <v>66</v>
       </c>
@@ -1864,7 +1829,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A2" s="4" t="s">
         <v>26</v>
       </c>
@@ -1872,7 +1837,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A3" s="3" t="s">
         <v>29</v>
       </c>
@@ -1880,7 +1845,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A4" s="3" t="s">
         <v>17</v>
       </c>

</xml_diff>